<commit_message>
40% of bridges have a length and condition, first map of the N1
</commit_message>
<xml_diff>
--- a/EPA1352-G11-A2/check_N1_df.xlsx
+++ b/EPA1352-G11-A2/check_N1_df.xlsx
@@ -516,7 +516,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -600,7 +600,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -642,7 +642,7 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -684,7 +684,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,7 +768,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -810,7 +810,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -852,7 +852,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -894,7 +894,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -936,7 +936,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -978,7 +978,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1020,7 +1020,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1062,7 +1062,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1202,7 +1202,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1244,7 +1244,7 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1286,7 +1286,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1472,7 +1472,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1604,7 +1604,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1750,7 +1750,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1792,7 +1792,7 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1882,7 +1882,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1924,7 +1924,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2008,7 +2008,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2050,7 +2050,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2184,7 +2184,7 @@
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2416,7 +2416,7 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2562,7 +2562,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2700,7 +2700,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2742,7 +2742,7 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2882,7 +2882,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2966,7 +2966,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3198,7 +3198,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3288,7 +3288,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3378,7 +3378,7 @@
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -3420,7 +3420,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -3558,7 +3558,7 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3648,7 +3648,7 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3836,7 +3836,7 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3982,7 +3982,7 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -4214,7 +4214,7 @@
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4256,7 +4256,7 @@
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -4390,7 +4390,7 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4480,7 +4480,7 @@
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -4668,7 +4668,7 @@
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -4710,7 +4710,7 @@
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -4892,7 +4892,7 @@
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -4982,7 +4982,7 @@
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -5024,7 +5024,7 @@
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -5108,7 +5108,7 @@
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Others / Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -5150,7 +5150,7 @@
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -5284,7 +5284,7 @@
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -5368,7 +5368,7 @@
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -5410,7 +5410,7 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -5452,7 +5452,7 @@
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -5586,7 +5586,7 @@
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -5628,7 +5628,7 @@
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -5670,7 +5670,7 @@
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -5754,7 +5754,7 @@
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -5796,7 +5796,7 @@
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -5838,7 +5838,7 @@
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -5922,7 +5922,7 @@
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -5964,7 +5964,7 @@
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -6006,7 +6006,7 @@
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -6140,7 +6140,7 @@
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -6182,7 +6182,7 @@
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -6316,7 +6316,7 @@
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -6358,7 +6358,7 @@
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -6442,7 +6442,7 @@
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -6484,7 +6484,7 @@
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -6526,7 +6526,7 @@
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -6568,7 +6568,7 @@
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -6708,7 +6708,7 @@
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -6750,7 +6750,7 @@
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -6792,7 +6792,7 @@
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
@@ -6876,7 +6876,7 @@
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
@@ -6918,7 +6918,7 @@
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -7002,7 +7002,7 @@
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
@@ -7044,7 +7044,7 @@
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -7086,7 +7086,7 @@
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
@@ -7128,7 +7128,7 @@
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
@@ -7254,7 +7254,7 @@
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -7296,7 +7296,7 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -7338,7 +7338,7 @@
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -7422,7 +7422,7 @@
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
@@ -7464,7 +7464,7 @@
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -7554,7 +7554,7 @@
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -7596,7 +7596,7 @@
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
@@ -7638,7 +7638,7 @@
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -7680,7 +7680,7 @@
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -7722,7 +7722,7 @@
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -7764,7 +7764,7 @@
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -7904,7 +7904,7 @@
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -7946,7 +7946,7 @@
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -7988,7 +7988,7 @@
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -8078,7 +8078,7 @@
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
@@ -8168,7 +8168,7 @@
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -8210,7 +8210,7 @@
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -8252,7 +8252,7 @@
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
@@ -8294,7 +8294,7 @@
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -8384,7 +8384,7 @@
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
@@ -8426,7 +8426,7 @@
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
@@ -8468,7 +8468,7 @@
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
@@ -8552,7 +8552,7 @@
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
@@ -8642,7 +8642,7 @@
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -8684,7 +8684,7 @@
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -8768,7 +8768,7 @@
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -8810,7 +8810,7 @@
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
@@ -8852,7 +8852,7 @@
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
@@ -8894,7 +8894,7 @@
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
@@ -8936,7 +8936,7 @@
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
@@ -8978,7 +8978,7 @@
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
@@ -9112,7 +9112,7 @@
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -9154,7 +9154,7 @@
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -9196,7 +9196,7 @@
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -9238,7 +9238,7 @@
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -9280,7 +9280,7 @@
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
@@ -9414,7 +9414,7 @@
       <c r="G204" t="inlineStr"/>
       <c r="H204" t="inlineStr">
         <is>
-          <t>RailRoadCrossing</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
@@ -9456,7 +9456,7 @@
       <c r="G205" t="inlineStr"/>
       <c r="H205" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -9498,7 +9498,7 @@
       <c r="G206" t="inlineStr"/>
       <c r="H206" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
@@ -9540,7 +9540,7 @@
       <c r="G207" t="inlineStr"/>
       <c r="H207" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
@@ -9674,7 +9674,7 @@
       <c r="G210" t="inlineStr"/>
       <c r="H210" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -9716,7 +9716,7 @@
       <c r="G211" t="inlineStr"/>
       <c r="H211" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
@@ -9758,7 +9758,7 @@
       <c r="G212" t="inlineStr"/>
       <c r="H212" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
@@ -9848,7 +9848,7 @@
       <c r="G214" t="inlineStr"/>
       <c r="H214" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
@@ -9982,7 +9982,7 @@
       <c r="G217" t="inlineStr"/>
       <c r="H217" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I217" t="inlineStr">
@@ -10024,7 +10024,7 @@
       <c r="G218" t="inlineStr"/>
       <c r="H218" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -10198,7 +10198,7 @@
       <c r="G222" t="inlineStr"/>
       <c r="H222" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -10332,7 +10332,7 @@
       <c r="G225" t="inlineStr"/>
       <c r="H225" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
@@ -10374,7 +10374,7 @@
       <c r="G226" t="inlineStr"/>
       <c r="H226" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
@@ -10464,7 +10464,7 @@
       <c r="G228" t="inlineStr"/>
       <c r="H228" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
@@ -10604,7 +10604,7 @@
       <c r="G231" t="inlineStr"/>
       <c r="H231" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I231" t="inlineStr">
@@ -10688,7 +10688,7 @@
       <c r="G233" t="inlineStr"/>
       <c r="H233" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
@@ -10730,7 +10730,7 @@
       <c r="G234" t="inlineStr"/>
       <c r="H234" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -10864,7 +10864,7 @@
       <c r="G237" t="inlineStr"/>
       <c r="H237" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
@@ -10906,7 +10906,7 @@
       <c r="G238" t="inlineStr"/>
       <c r="H238" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
@@ -10948,7 +10948,7 @@
       <c r="G239" t="inlineStr"/>
       <c r="H239" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -11088,7 +11088,7 @@
       <c r="G242" t="inlineStr"/>
       <c r="H242" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -11270,7 +11270,7 @@
       <c r="G246" t="inlineStr"/>
       <c r="H246" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -11360,7 +11360,7 @@
       <c r="G248" t="inlineStr"/>
       <c r="H248" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
@@ -11500,7 +11500,7 @@
       <c r="G251" t="inlineStr"/>
       <c r="H251" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -11590,7 +11590,7 @@
       <c r="G253" t="inlineStr"/>
       <c r="H253" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -11674,7 +11674,7 @@
       <c r="G255" t="inlineStr"/>
       <c r="H255" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -11716,7 +11716,7 @@
       <c r="G256" t="inlineStr"/>
       <c r="H256" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -11890,7 +11890,7 @@
       <c r="G260" t="inlineStr"/>
       <c r="H260" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
@@ -11980,7 +11980,7 @@
       <c r="G262" t="inlineStr"/>
       <c r="H262" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
@@ -12210,7 +12210,7 @@
       <c r="G267" t="inlineStr"/>
       <c r="H267" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I267" t="inlineStr">
@@ -12348,7 +12348,7 @@
       <c r="G270" t="inlineStr"/>
       <c r="H270" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I270" t="inlineStr">
@@ -12480,7 +12480,7 @@
       <c r="G273" t="inlineStr"/>
       <c r="H273" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I273" t="inlineStr">
@@ -12522,7 +12522,7 @@
       <c r="G274" t="inlineStr"/>
       <c r="H274" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
@@ -12606,7 +12606,7 @@
       <c r="G276" t="inlineStr"/>
       <c r="H276" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I276" t="inlineStr">
@@ -12696,7 +12696,7 @@
       <c r="G278" t="inlineStr"/>
       <c r="H278" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I278" t="inlineStr">
@@ -12786,7 +12786,7 @@
       <c r="G280" t="inlineStr"/>
       <c r="H280" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I280" t="inlineStr">
@@ -12876,7 +12876,7 @@
       <c r="G282" t="inlineStr"/>
       <c r="H282" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I282" t="inlineStr">
@@ -13016,7 +13016,7 @@
       <c r="G285" t="inlineStr"/>
       <c r="H285" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I285" t="inlineStr">
@@ -13106,7 +13106,7 @@
       <c r="G287" t="inlineStr"/>
       <c r="H287" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I287" t="inlineStr">
@@ -13246,7 +13246,7 @@
       <c r="G290" t="inlineStr"/>
       <c r="H290" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I290" t="inlineStr">
@@ -13336,7 +13336,7 @@
       <c r="G292" t="inlineStr"/>
       <c r="H292" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I292" t="inlineStr">
@@ -13378,7 +13378,7 @@
       <c r="G293" t="inlineStr"/>
       <c r="H293" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I293" t="inlineStr">
@@ -13462,7 +13462,7 @@
       <c r="G295" t="inlineStr"/>
       <c r="H295" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I295" t="inlineStr">
@@ -13552,7 +13552,7 @@
       <c r="G297" t="inlineStr"/>
       <c r="H297" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I297" t="inlineStr">
@@ -13642,7 +13642,7 @@
       <c r="G299" t="inlineStr"/>
       <c r="H299" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I299" t="inlineStr">
@@ -13774,7 +13774,7 @@
       <c r="G302" t="inlineStr"/>
       <c r="H302" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I302" t="inlineStr">
@@ -13864,7 +13864,7 @@
       <c r="G304" t="inlineStr"/>
       <c r="H304" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I304" t="inlineStr">
@@ -13906,7 +13906,7 @@
       <c r="G305" t="inlineStr"/>
       <c r="H305" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I305" t="inlineStr">
@@ -14038,7 +14038,7 @@
       <c r="G308" t="inlineStr"/>
       <c r="H308" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I308" t="inlineStr">
@@ -14176,7 +14176,7 @@
       <c r="G311" t="inlineStr"/>
       <c r="H311" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I311" t="inlineStr">
@@ -14266,7 +14266,7 @@
       <c r="G313" t="inlineStr"/>
       <c r="H313" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I313" t="inlineStr">
@@ -14442,7 +14442,7 @@
       <c r="G317" t="inlineStr"/>
       <c r="H317" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I317" t="inlineStr">
@@ -14532,7 +14532,7 @@
       <c r="G319" t="inlineStr"/>
       <c r="H319" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
@@ -14574,7 +14574,7 @@
       <c r="G320" t="inlineStr"/>
       <c r="H320" t="inlineStr">
         <is>
-          <t>Others / Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I320" t="inlineStr">
@@ -14658,7 +14658,7 @@
       <c r="G322" t="inlineStr"/>
       <c r="H322" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
@@ -14700,7 +14700,7 @@
       <c r="G323" t="inlineStr"/>
       <c r="H323" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I323" t="inlineStr">
@@ -14742,7 +14742,7 @@
       <c r="G324" t="inlineStr"/>
       <c r="H324" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I324" t="inlineStr">
@@ -14784,7 +14784,7 @@
       <c r="G325" t="inlineStr"/>
       <c r="H325" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I325" t="inlineStr">
@@ -14826,7 +14826,7 @@
       <c r="G326" t="inlineStr"/>
       <c r="H326" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I326" t="inlineStr">
@@ -14910,7 +14910,7 @@
       <c r="G328" t="inlineStr"/>
       <c r="H328" t="inlineStr">
         <is>
-          <t>RailRoadCrossing</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I328" t="inlineStr">
@@ -14952,7 +14952,7 @@
       <c r="G329" t="inlineStr"/>
       <c r="H329" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I329" t="inlineStr">
@@ -15042,7 +15042,7 @@
       <c r="G331" t="inlineStr"/>
       <c r="H331" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I331" t="inlineStr">
@@ -15084,7 +15084,7 @@
       <c r="G332" t="inlineStr"/>
       <c r="H332" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I332" t="inlineStr">
@@ -15126,7 +15126,7 @@
       <c r="G333" t="inlineStr"/>
       <c r="H333" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I333" t="inlineStr">
@@ -15252,7 +15252,7 @@
       <c r="G336" t="inlineStr"/>
       <c r="H336" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I336" t="inlineStr">
@@ -15294,7 +15294,7 @@
       <c r="G337" t="inlineStr"/>
       <c r="H337" t="inlineStr">
         <is>
-          <t>CrossRoad / KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I337" t="inlineStr">
@@ -15336,7 +15336,7 @@
       <c r="G338" t="inlineStr"/>
       <c r="H338" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I338" t="inlineStr">
@@ -15378,7 +15378,7 @@
       <c r="G339" t="inlineStr"/>
       <c r="H339" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I339" t="inlineStr">
@@ -15512,7 +15512,7 @@
       <c r="G342" t="inlineStr"/>
       <c r="H342" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I342" t="inlineStr">
@@ -15554,7 +15554,7 @@
       <c r="G343" t="inlineStr"/>
       <c r="H343" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I343" t="inlineStr">
@@ -15596,7 +15596,7 @@
       <c r="G344" t="inlineStr"/>
       <c r="H344" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I344" t="inlineStr">
@@ -15638,7 +15638,7 @@
       <c r="G345" t="inlineStr"/>
       <c r="H345" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I345" t="inlineStr">
@@ -15680,7 +15680,7 @@
       <c r="G346" t="inlineStr"/>
       <c r="H346" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I346" t="inlineStr">
@@ -15722,7 +15722,7 @@
       <c r="G347" t="inlineStr"/>
       <c r="H347" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I347" t="inlineStr">
@@ -15764,7 +15764,7 @@
       <c r="G348" t="inlineStr"/>
       <c r="H348" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -15898,7 +15898,7 @@
       <c r="G351" t="inlineStr"/>
       <c r="H351" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I351" t="inlineStr">
@@ -15940,7 +15940,7 @@
       <c r="G352" t="inlineStr"/>
       <c r="H352" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I352" t="inlineStr">
@@ -15982,7 +15982,7 @@
       <c r="G353" t="inlineStr"/>
       <c r="H353" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I353" t="inlineStr">
@@ -16024,7 +16024,7 @@
       <c r="G354" t="inlineStr"/>
       <c r="H354" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I354" t="inlineStr">
@@ -16066,7 +16066,7 @@
       <c r="G355" t="inlineStr"/>
       <c r="H355" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I355" t="inlineStr">
@@ -16108,7 +16108,7 @@
       <c r="G356" t="inlineStr"/>
       <c r="H356" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I356" t="inlineStr">
@@ -16150,7 +16150,7 @@
       <c r="G357" t="inlineStr"/>
       <c r="H357" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I357" t="inlineStr">
@@ -16192,7 +16192,7 @@
       <c r="G358" t="inlineStr"/>
       <c r="H358" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I358" t="inlineStr">
@@ -16326,7 +16326,7 @@
       <c r="G361" t="inlineStr"/>
       <c r="H361" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I361" t="inlineStr">
@@ -16368,7 +16368,7 @@
       <c r="G362" t="inlineStr"/>
       <c r="H362" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I362" t="inlineStr">
@@ -16410,7 +16410,7 @@
       <c r="G363" t="inlineStr"/>
       <c r="H363" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I363" t="inlineStr">
@@ -16452,7 +16452,7 @@
       <c r="G364" t="inlineStr"/>
       <c r="H364" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I364" t="inlineStr">
@@ -16494,7 +16494,7 @@
       <c r="G365" t="inlineStr"/>
       <c r="H365" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I365" t="inlineStr">
@@ -16536,7 +16536,7 @@
       <c r="G366" t="inlineStr"/>
       <c r="H366" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I366" t="inlineStr">
@@ -16670,7 +16670,7 @@
       <c r="G369" t="inlineStr"/>
       <c r="H369" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I369" t="inlineStr">
@@ -16760,7 +16760,7 @@
       <c r="G371" t="inlineStr"/>
       <c r="H371" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I371" t="inlineStr">
@@ -16802,7 +16802,7 @@
       <c r="G372" t="inlineStr"/>
       <c r="H372" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I372" t="inlineStr">
@@ -16844,7 +16844,7 @@
       <c r="G373" t="inlineStr"/>
       <c r="H373" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I373" t="inlineStr">
@@ -16886,7 +16886,7 @@
       <c r="G374" t="inlineStr"/>
       <c r="H374" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I374" t="inlineStr">
@@ -16970,7 +16970,7 @@
       <c r="G376" t="inlineStr"/>
       <c r="H376" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I376" t="inlineStr">
@@ -17108,7 +17108,7 @@
       <c r="G379" t="inlineStr"/>
       <c r="H379" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I379" t="inlineStr">
@@ -17246,7 +17246,7 @@
       <c r="G382" t="inlineStr"/>
       <c r="H382" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I382" t="inlineStr">
@@ -17384,7 +17384,7 @@
       <c r="G385" t="inlineStr"/>
       <c r="H385" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I385" t="inlineStr">
@@ -17522,7 +17522,7 @@
       <c r="G388" t="inlineStr"/>
       <c r="H388" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I388" t="inlineStr">
@@ -17752,7 +17752,7 @@
       <c r="G393" t="inlineStr"/>
       <c r="H393" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I393" t="inlineStr">
@@ -17836,7 +17836,7 @@
       <c r="G395" t="inlineStr"/>
       <c r="H395" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I395" t="inlineStr">
@@ -17920,7 +17920,7 @@
       <c r="G397" t="inlineStr"/>
       <c r="H397" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I397" t="inlineStr">
@@ -17962,7 +17962,7 @@
       <c r="G398" t="inlineStr"/>
       <c r="H398" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I398" t="inlineStr">
@@ -18130,7 +18130,7 @@
       <c r="G402" t="inlineStr"/>
       <c r="H402" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I402" t="inlineStr">
@@ -18220,7 +18220,7 @@
       <c r="G404" t="inlineStr"/>
       <c r="H404" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I404" t="inlineStr">
@@ -18352,7 +18352,7 @@
       <c r="G407" t="inlineStr"/>
       <c r="H407" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I407" t="inlineStr">
@@ -18436,7 +18436,7 @@
       <c r="G409" t="inlineStr"/>
       <c r="H409" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I409" t="inlineStr">
@@ -18526,7 +18526,7 @@
       <c r="G411" t="inlineStr"/>
       <c r="H411" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I411" t="inlineStr">
@@ -18610,7 +18610,7 @@
       <c r="G413" t="inlineStr"/>
       <c r="H413" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I413" t="inlineStr">
@@ -18742,7 +18742,7 @@
       <c r="G416" t="inlineStr"/>
       <c r="H416" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I416" t="inlineStr">
@@ -18832,7 +18832,7 @@
       <c r="G418" t="inlineStr"/>
       <c r="H418" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I418" t="inlineStr">
@@ -18978,7 +18978,7 @@
       <c r="G421" t="inlineStr"/>
       <c r="H421" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I421" t="inlineStr">
@@ -19062,7 +19062,7 @@
       <c r="G423" t="inlineStr"/>
       <c r="H423" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I423" t="inlineStr">
@@ -19146,7 +19146,7 @@
       <c r="G425" t="inlineStr"/>
       <c r="H425" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I425" t="inlineStr">
@@ -19236,7 +19236,7 @@
       <c r="G427" t="inlineStr"/>
       <c r="H427" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I427" t="inlineStr">
@@ -19326,7 +19326,7 @@
       <c r="G429" t="inlineStr"/>
       <c r="H429" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I429" t="inlineStr">
@@ -19452,7 +19452,7 @@
       <c r="G432" t="inlineStr"/>
       <c r="H432" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I432" t="inlineStr">
@@ -19584,7 +19584,7 @@
       <c r="G435" t="inlineStr"/>
       <c r="H435" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I435" t="inlineStr">
@@ -19758,7 +19758,7 @@
       <c r="G439" t="inlineStr"/>
       <c r="H439" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I439" t="inlineStr">
@@ -19848,7 +19848,7 @@
       <c r="G441" t="inlineStr"/>
       <c r="H441" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I441" t="inlineStr">
@@ -19980,7 +19980,7 @@
       <c r="G444" t="inlineStr"/>
       <c r="H444" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I444" t="inlineStr">
@@ -20118,7 +20118,7 @@
       <c r="G447" t="inlineStr"/>
       <c r="H447" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I447" t="inlineStr">
@@ -20160,7 +20160,7 @@
       <c r="G448" t="inlineStr"/>
       <c r="H448" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I448" t="inlineStr">
@@ -20286,7 +20286,7 @@
       <c r="G451" t="inlineStr"/>
       <c r="H451" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I451" t="inlineStr">
@@ -20424,7 +20424,7 @@
       <c r="G454" t="inlineStr"/>
       <c r="H454" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I454" t="inlineStr">
@@ -20550,7 +20550,7 @@
       <c r="G457" t="inlineStr"/>
       <c r="H457" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I457" t="inlineStr">
@@ -20688,7 +20688,7 @@
       <c r="G460" t="inlineStr"/>
       <c r="H460" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I460" t="inlineStr">
@@ -20778,7 +20778,7 @@
       <c r="G462" t="inlineStr"/>
       <c r="H462" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I462" t="inlineStr">
@@ -20916,7 +20916,7 @@
       <c r="G465" t="inlineStr"/>
       <c r="H465" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I465" t="inlineStr">
@@ -21182,7 +21182,7 @@
       <c r="G471" t="inlineStr"/>
       <c r="H471" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I471" t="inlineStr">
@@ -21314,7 +21314,7 @@
       <c r="G474" t="inlineStr"/>
       <c r="H474" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I474" t="inlineStr">
@@ -21404,7 +21404,7 @@
       <c r="G476" t="inlineStr"/>
       <c r="H476" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I476" t="inlineStr">
@@ -21620,7 +21620,7 @@
       <c r="G481" t="inlineStr"/>
       <c r="H481" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
@@ -21710,7 +21710,7 @@
       <c r="G483" t="inlineStr"/>
       <c r="H483" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I483" t="inlineStr">
@@ -21850,7 +21850,7 @@
       <c r="G486" t="inlineStr"/>
       <c r="H486" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I486" t="inlineStr">
@@ -21934,7 +21934,7 @@
       <c r="G488" t="inlineStr"/>
       <c r="H488" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I488" t="inlineStr">
@@ -22080,7 +22080,7 @@
       <c r="G491" t="inlineStr"/>
       <c r="H491" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I491" t="inlineStr">
@@ -22304,7 +22304,7 @@
       <c r="G496" t="inlineStr"/>
       <c r="H496" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I496" t="inlineStr">
@@ -22346,7 +22346,7 @@
       <c r="G497" t="inlineStr"/>
       <c r="H497" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I497" t="inlineStr">
@@ -22492,7 +22492,7 @@
       <c r="G500" t="inlineStr"/>
       <c r="H500" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I500" t="inlineStr">
@@ -22582,7 +22582,7 @@
       <c r="G502" t="inlineStr"/>
       <c r="H502" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I502" t="inlineStr">
@@ -22672,7 +22672,7 @@
       <c r="G504" t="inlineStr"/>
       <c r="H504" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I504" t="inlineStr">
@@ -22806,7 +22806,7 @@
       <c r="G507" t="inlineStr"/>
       <c r="H507" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I507" t="inlineStr">
@@ -23080,7 +23080,7 @@
       <c r="G513" t="inlineStr"/>
       <c r="H513" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I513" t="inlineStr">
@@ -23360,7 +23360,7 @@
       <c r="G519" t="inlineStr"/>
       <c r="H519" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I519" t="inlineStr">
@@ -23500,7 +23500,7 @@
       <c r="G522" t="inlineStr"/>
       <c r="H522" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I522" t="inlineStr">
@@ -23590,7 +23590,7 @@
       <c r="G524" t="inlineStr"/>
       <c r="H524" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I524" t="inlineStr">
@@ -23772,7 +23772,7 @@
       <c r="G528" t="inlineStr"/>
       <c r="H528" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I528" t="inlineStr">
@@ -23856,7 +23856,7 @@
       <c r="G530" t="inlineStr"/>
       <c r="H530" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I530" t="inlineStr">
@@ -23898,7 +23898,7 @@
       <c r="G531" t="inlineStr"/>
       <c r="H531" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I531" t="inlineStr">
@@ -24038,7 +24038,7 @@
       <c r="G534" t="inlineStr"/>
       <c r="H534" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I534" t="inlineStr">
@@ -24080,7 +24080,7 @@
       <c r="G535" t="inlineStr"/>
       <c r="H535" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I535" t="inlineStr">
@@ -24226,7 +24226,7 @@
       <c r="G538" t="inlineStr"/>
       <c r="H538" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I538" t="inlineStr">
@@ -24402,7 +24402,7 @@
       <c r="G542" t="inlineStr"/>
       <c r="H542" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I542" t="inlineStr">
@@ -24444,7 +24444,7 @@
       <c r="G543" t="inlineStr"/>
       <c r="H543" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I543" t="inlineStr">
@@ -24578,7 +24578,7 @@
       <c r="G546" t="inlineStr"/>
       <c r="H546" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I546" t="inlineStr">
@@ -24620,7 +24620,7 @@
       <c r="G547" t="inlineStr"/>
       <c r="H547" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I547" t="inlineStr">
@@ -24704,7 +24704,7 @@
       <c r="G549" t="inlineStr"/>
       <c r="H549" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I549" t="inlineStr">
@@ -24746,7 +24746,7 @@
       <c r="G550" t="inlineStr"/>
       <c r="H550" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I550" t="inlineStr">
@@ -24788,7 +24788,7 @@
       <c r="G551" t="inlineStr"/>
       <c r="H551" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I551" t="inlineStr">
@@ -24928,7 +24928,7 @@
       <c r="G554" t="inlineStr"/>
       <c r="H554" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I554" t="inlineStr">
@@ -24970,7 +24970,7 @@
       <c r="G555" t="inlineStr"/>
       <c r="H555" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I555" t="inlineStr">
@@ -25146,7 +25146,7 @@
       <c r="G559" t="inlineStr"/>
       <c r="H559" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I559" t="inlineStr">
@@ -25236,7 +25236,7 @@
       <c r="G561" t="inlineStr"/>
       <c r="H561" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I561" t="inlineStr">
@@ -25376,7 +25376,7 @@
       <c r="G564" t="inlineStr"/>
       <c r="H564" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I564" t="inlineStr">
@@ -25418,7 +25418,7 @@
       <c r="G565" t="inlineStr"/>
       <c r="H565" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I565" t="inlineStr">
@@ -25460,7 +25460,7 @@
       <c r="G566" t="inlineStr"/>
       <c r="H566" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I566" t="inlineStr">
@@ -25502,7 +25502,7 @@
       <c r="G567" t="inlineStr"/>
       <c r="H567" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I567" t="inlineStr">
@@ -25544,7 +25544,7 @@
       <c r="G568" t="inlineStr"/>
       <c r="H568" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I568" t="inlineStr">
@@ -25634,7 +25634,7 @@
       <c r="G570" t="inlineStr"/>
       <c r="H570" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I570" t="inlineStr">
@@ -25780,7 +25780,7 @@
       <c r="G573" t="inlineStr"/>
       <c r="H573" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I573" t="inlineStr">
@@ -25920,7 +25920,7 @@
       <c r="G576" t="inlineStr"/>
       <c r="H576" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I576" t="inlineStr">
@@ -26152,7 +26152,7 @@
       <c r="G581" t="inlineStr"/>
       <c r="H581" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I581" t="inlineStr">
@@ -26242,7 +26242,7 @@
       <c r="G583" t="inlineStr"/>
       <c r="H583" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I583" t="inlineStr">
@@ -26424,7 +26424,7 @@
       <c r="G587" t="inlineStr"/>
       <c r="H587" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I587" t="inlineStr">
@@ -26466,7 +26466,7 @@
       <c r="G588" t="inlineStr"/>
       <c r="H588" t="inlineStr">
         <is>
-          <t>SideRoad,Right / SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I588" t="inlineStr">
@@ -26508,7 +26508,7 @@
       <c r="G589" t="inlineStr"/>
       <c r="H589" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I589" t="inlineStr">
@@ -26592,7 +26592,7 @@
       <c r="G591" t="inlineStr"/>
       <c r="H591" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I591" t="inlineStr">
@@ -26724,7 +26724,7 @@
       <c r="G594" t="inlineStr"/>
       <c r="H594" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I594" t="inlineStr">
@@ -26814,7 +26814,7 @@
       <c r="G596" t="inlineStr"/>
       <c r="H596" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I596" t="inlineStr">
@@ -26856,7 +26856,7 @@
       <c r="G597" t="inlineStr"/>
       <c r="H597" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I597" t="inlineStr">
@@ -27024,7 +27024,7 @@
       <c r="G601" t="inlineStr"/>
       <c r="H601" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I601" t="inlineStr">
@@ -27156,7 +27156,7 @@
       <c r="G604" t="inlineStr"/>
       <c r="H604" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I604" t="inlineStr">
@@ -27198,7 +27198,7 @@
       <c r="G605" t="inlineStr"/>
       <c r="H605" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I605" t="inlineStr">
@@ -27240,7 +27240,7 @@
       <c r="G606" t="inlineStr"/>
       <c r="H606" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I606" t="inlineStr">
@@ -27330,7 +27330,7 @@
       <c r="G608" t="inlineStr"/>
       <c r="H608" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I608" t="inlineStr">
@@ -27414,7 +27414,7 @@
       <c r="G610" t="inlineStr"/>
       <c r="H610" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I610" t="inlineStr">
@@ -27498,7 +27498,7 @@
       <c r="G612" t="inlineStr"/>
       <c r="H612" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I612" t="inlineStr">
@@ -27540,7 +27540,7 @@
       <c r="G613" t="inlineStr"/>
       <c r="H613" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I613" t="inlineStr">
@@ -27672,7 +27672,7 @@
       <c r="G616" t="inlineStr"/>
       <c r="H616" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I616" t="inlineStr">
@@ -27714,7 +27714,7 @@
       <c r="G617" t="inlineStr"/>
       <c r="H617" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I617" t="inlineStr">
@@ -27804,7 +27804,7 @@
       <c r="G619" t="inlineStr"/>
       <c r="H619" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I619" t="inlineStr">
@@ -27846,7 +27846,7 @@
       <c r="G620" t="inlineStr"/>
       <c r="H620" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I620" t="inlineStr">
@@ -27930,7 +27930,7 @@
       <c r="G622" t="inlineStr"/>
       <c r="H622" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I622" t="inlineStr">
@@ -27972,7 +27972,7 @@
       <c r="G623" t="inlineStr"/>
       <c r="H623" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I623" t="inlineStr">
@@ -28118,7 +28118,7 @@
       <c r="G626" t="inlineStr"/>
       <c r="H626" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I626" t="inlineStr">
@@ -28160,7 +28160,7 @@
       <c r="G627" t="inlineStr"/>
       <c r="H627" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I627" t="inlineStr">
@@ -28250,7 +28250,7 @@
       <c r="G629" t="inlineStr"/>
       <c r="H629" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I629" t="inlineStr">
@@ -28292,7 +28292,7 @@
       <c r="G630" t="inlineStr"/>
       <c r="H630" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I630" t="inlineStr">
@@ -28334,7 +28334,7 @@
       <c r="G631" t="inlineStr"/>
       <c r="H631" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I631" t="inlineStr">
@@ -28424,7 +28424,7 @@
       <c r="G633" t="inlineStr"/>
       <c r="H633" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I633" t="inlineStr">
@@ -28466,7 +28466,7 @@
       <c r="G634" t="inlineStr"/>
       <c r="H634" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I634" t="inlineStr">
@@ -28606,7 +28606,7 @@
       <c r="G637" t="inlineStr"/>
       <c r="H637" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I637" t="inlineStr">
@@ -28648,7 +28648,7 @@
       <c r="G638" t="inlineStr"/>
       <c r="H638" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I638" t="inlineStr">
@@ -28738,7 +28738,7 @@
       <c r="G640" t="inlineStr"/>
       <c r="H640" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I640" t="inlineStr">
@@ -28870,7 +28870,7 @@
       <c r="G643" t="inlineStr"/>
       <c r="H643" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I643" t="inlineStr">
@@ -29058,7 +29058,7 @@
       <c r="G647" t="inlineStr"/>
       <c r="H647" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I647" t="inlineStr">
@@ -29184,7 +29184,7 @@
       <c r="G650" t="inlineStr"/>
       <c r="H650" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I650" t="inlineStr">
@@ -29268,7 +29268,7 @@
       <c r="G652" t="inlineStr"/>
       <c r="H652" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I652" t="inlineStr">
@@ -29394,7 +29394,7 @@
       <c r="G655" t="inlineStr"/>
       <c r="H655" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I655" t="inlineStr">
@@ -29576,7 +29576,7 @@
       <c r="G659" t="inlineStr"/>
       <c r="H659" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I659" t="inlineStr">
@@ -29752,7 +29752,7 @@
       <c r="G663" t="inlineStr"/>
       <c r="H663" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I663" t="inlineStr">
@@ -29836,7 +29836,7 @@
       <c r="G665" t="inlineStr"/>
       <c r="H665" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I665" t="inlineStr">
@@ -29878,7 +29878,7 @@
       <c r="G666" t="inlineStr"/>
       <c r="H666" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I666" t="inlineStr">
@@ -30110,7 +30110,7 @@
       <c r="G671" t="inlineStr"/>
       <c r="H671" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I671" t="inlineStr">
@@ -30152,7 +30152,7 @@
       <c r="G672" t="inlineStr"/>
       <c r="H672" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I672" t="inlineStr">
@@ -30194,7 +30194,7 @@
       <c r="G673" t="inlineStr"/>
       <c r="H673" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I673" t="inlineStr">
@@ -30236,7 +30236,7 @@
       <c r="G674" t="inlineStr"/>
       <c r="H674" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I674" t="inlineStr">
@@ -30278,7 +30278,7 @@
       <c r="G675" t="inlineStr"/>
       <c r="H675" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I675" t="inlineStr">
@@ -30368,7 +30368,7 @@
       <c r="G677" t="inlineStr"/>
       <c r="H677" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I677" t="inlineStr">
@@ -30410,7 +30410,7 @@
       <c r="G678" t="inlineStr"/>
       <c r="H678" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I678" t="inlineStr">
@@ -30452,7 +30452,7 @@
       <c r="G679" t="inlineStr"/>
       <c r="H679" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I679" t="inlineStr">
@@ -30592,7 +30592,7 @@
       <c r="G682" t="inlineStr"/>
       <c r="H682" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I682" t="inlineStr">
@@ -30732,7 +30732,7 @@
       <c r="G685" t="inlineStr"/>
       <c r="H685" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I685" t="inlineStr">
@@ -30774,7 +30774,7 @@
       <c r="G686" t="inlineStr"/>
       <c r="H686" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I686" t="inlineStr">
@@ -30906,7 +30906,7 @@
       <c r="G689" t="inlineStr"/>
       <c r="H689" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I689" t="inlineStr">
@@ -31132,7 +31132,7 @@
       <c r="G694" t="inlineStr"/>
       <c r="H694" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I694" t="inlineStr">
@@ -31264,7 +31264,7 @@
       <c r="G697" t="inlineStr"/>
       <c r="H697" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I697" t="inlineStr">
@@ -31354,7 +31354,7 @@
       <c r="G699" t="inlineStr"/>
       <c r="H699" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I699" t="inlineStr">
@@ -31396,7 +31396,7 @@
       <c r="G700" t="inlineStr"/>
       <c r="H700" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I700" t="inlineStr">
@@ -31480,7 +31480,7 @@
       <c r="G702" t="inlineStr"/>
       <c r="H702" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I702" t="inlineStr">
@@ -31522,7 +31522,7 @@
       <c r="G703" t="inlineStr"/>
       <c r="H703" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I703" t="inlineStr">
@@ -31612,7 +31612,7 @@
       <c r="G705" t="inlineStr"/>
       <c r="H705" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I705" t="inlineStr">
@@ -31654,7 +31654,7 @@
       <c r="G706" t="inlineStr"/>
       <c r="H706" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I706" t="inlineStr">
@@ -31744,7 +31744,7 @@
       <c r="G708" t="inlineStr"/>
       <c r="H708" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I708" t="inlineStr">
@@ -31828,7 +31828,7 @@
       <c r="G710" t="inlineStr"/>
       <c r="H710" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I710" t="inlineStr">
@@ -31968,7 +31968,7 @@
       <c r="G713" t="inlineStr"/>
       <c r="H713" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I713" t="inlineStr">
@@ -32156,7 +32156,7 @@
       <c r="G717" t="inlineStr"/>
       <c r="H717" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I717" t="inlineStr">
@@ -32294,7 +32294,7 @@
       <c r="G720" t="inlineStr"/>
       <c r="H720" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I720" t="inlineStr">
@@ -32384,7 +32384,7 @@
       <c r="G722" t="inlineStr"/>
       <c r="H722" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I722" t="inlineStr">
@@ -32468,7 +32468,7 @@
       <c r="G724" t="inlineStr"/>
       <c r="H724" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I724" t="inlineStr">
@@ -32558,7 +32558,7 @@
       <c r="G726" t="inlineStr"/>
       <c r="H726" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I726" t="inlineStr">
@@ -32690,7 +32690,7 @@
       <c r="G729" t="inlineStr"/>
       <c r="H729" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I729" t="inlineStr">
@@ -32774,7 +32774,7 @@
       <c r="G731" t="inlineStr"/>
       <c r="H731" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I731" t="inlineStr">
@@ -32864,7 +32864,7 @@
       <c r="G733" t="inlineStr"/>
       <c r="H733" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I733" t="inlineStr">
@@ -32954,7 +32954,7 @@
       <c r="G735" t="inlineStr"/>
       <c r="H735" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I735" t="inlineStr">
@@ -33086,7 +33086,7 @@
       <c r="G738" t="inlineStr"/>
       <c r="H738" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I738" t="inlineStr">
@@ -33316,7 +33316,7 @@
       <c r="G743" t="inlineStr"/>
       <c r="H743" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I743" t="inlineStr">
@@ -33504,7 +33504,7 @@
       <c r="G747" t="inlineStr"/>
       <c r="H747" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I747" t="inlineStr">
@@ -33734,7 +33734,7 @@
       <c r="G752" t="inlineStr"/>
       <c r="H752" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I752" t="inlineStr">
@@ -33776,7 +33776,7 @@
       <c r="G753" t="inlineStr"/>
       <c r="H753" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I753" t="inlineStr">
@@ -33818,7 +33818,7 @@
       <c r="G754" t="inlineStr"/>
       <c r="H754" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I754" t="inlineStr">
@@ -33902,7 +33902,7 @@
       <c r="G756" t="inlineStr"/>
       <c r="H756" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I756" t="inlineStr">
@@ -34084,7 +34084,7 @@
       <c r="G760" t="inlineStr"/>
       <c r="H760" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I760" t="inlineStr">
@@ -34266,7 +34266,7 @@
       <c r="G764" t="inlineStr"/>
       <c r="H764" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I764" t="inlineStr">
@@ -34356,7 +34356,7 @@
       <c r="G766" t="inlineStr"/>
       <c r="H766" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I766" t="inlineStr">
@@ -34488,7 +34488,7 @@
       <c r="G769" t="inlineStr"/>
       <c r="H769" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I769" t="inlineStr">
@@ -34620,7 +34620,7 @@
       <c r="G772" t="inlineStr"/>
       <c r="H772" t="inlineStr">
         <is>
-          <t>KmPost / KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I772" t="inlineStr">
@@ -34758,7 +34758,7 @@
       <c r="G775" t="inlineStr"/>
       <c r="H775" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I775" t="inlineStr">
@@ -34896,7 +34896,7 @@
       <c r="G778" t="inlineStr"/>
       <c r="H778" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I778" t="inlineStr">
@@ -34938,7 +34938,7 @@
       <c r="G779" t="inlineStr"/>
       <c r="H779" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I779" t="inlineStr">
@@ -34980,7 +34980,7 @@
       <c r="G780" t="inlineStr"/>
       <c r="H780" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I780" t="inlineStr">
@@ -35022,7 +35022,7 @@
       <c r="G781" t="inlineStr"/>
       <c r="H781" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I781" t="inlineStr">
@@ -35112,7 +35112,7 @@
       <c r="G783" t="inlineStr"/>
       <c r="H783" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I783" t="inlineStr">
@@ -35202,7 +35202,7 @@
       <c r="G785" t="inlineStr"/>
       <c r="H785" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I785" t="inlineStr">
@@ -35286,7 +35286,7 @@
       <c r="G787" t="inlineStr"/>
       <c r="H787" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I787" t="inlineStr">
@@ -35370,7 +35370,7 @@
       <c r="G789" t="inlineStr"/>
       <c r="H789" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I789" t="inlineStr">
@@ -35510,7 +35510,7 @@
       <c r="G792" t="inlineStr"/>
       <c r="H792" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I792" t="inlineStr">
@@ -35642,7 +35642,7 @@
       <c r="G795" t="inlineStr"/>
       <c r="H795" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I795" t="inlineStr">
@@ -35774,7 +35774,7 @@
       <c r="G798" t="inlineStr"/>
       <c r="H798" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I798" t="inlineStr">
@@ -35864,7 +35864,7 @@
       <c r="G800" t="inlineStr"/>
       <c r="H800" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I800" t="inlineStr">
@@ -35906,7 +35906,7 @@
       <c r="G801" t="inlineStr"/>
       <c r="H801" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I801" t="inlineStr">
@@ -36082,7 +36082,7 @@
       <c r="G805" t="inlineStr"/>
       <c r="H805" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I805" t="inlineStr">
@@ -36166,7 +36166,7 @@
       <c r="G807" t="inlineStr"/>
       <c r="H807" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I807" t="inlineStr">
@@ -36208,7 +36208,7 @@
       <c r="G808" t="inlineStr"/>
       <c r="H808" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I808" t="inlineStr">
@@ -36342,7 +36342,7 @@
       <c r="G811" t="inlineStr"/>
       <c r="H811" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I811" t="inlineStr">
@@ -36384,7 +36384,7 @@
       <c r="G812" t="inlineStr"/>
       <c r="H812" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I812" t="inlineStr">
@@ -36516,7 +36516,7 @@
       <c r="G815" t="inlineStr"/>
       <c r="H815" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I815" t="inlineStr">
@@ -36600,7 +36600,7 @@
       <c r="G817" t="inlineStr"/>
       <c r="H817" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I817" t="inlineStr">
@@ -36732,7 +36732,7 @@
       <c r="G820" t="inlineStr"/>
       <c r="H820" t="inlineStr">
         <is>
-          <t>CrossRoad</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I820" t="inlineStr">
@@ -36816,7 +36816,7 @@
       <c r="G822" t="inlineStr"/>
       <c r="H822" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I822" t="inlineStr">
@@ -36956,7 +36956,7 @@
       <c r="G825" t="inlineStr"/>
       <c r="H825" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I825" t="inlineStr">
@@ -36998,7 +36998,7 @@
       <c r="G826" t="inlineStr"/>
       <c r="H826" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I826" t="inlineStr">
@@ -37040,7 +37040,7 @@
       <c r="G827" t="inlineStr"/>
       <c r="H827" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I827" t="inlineStr">
@@ -37082,7 +37082,7 @@
       <c r="G828" t="inlineStr"/>
       <c r="H828" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I828" t="inlineStr">
@@ -37124,7 +37124,7 @@
       <c r="G829" t="inlineStr"/>
       <c r="H829" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I829" t="inlineStr">
@@ -37214,7 +37214,7 @@
       <c r="G831" t="inlineStr"/>
       <c r="H831" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I831" t="inlineStr">
@@ -37438,7 +37438,7 @@
       <c r="G836" t="inlineStr"/>
       <c r="H836" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I836" t="inlineStr">
@@ -37528,7 +37528,7 @@
       <c r="G838" t="inlineStr"/>
       <c r="H838" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I838" t="inlineStr">
@@ -37570,7 +37570,7 @@
       <c r="G839" t="inlineStr"/>
       <c r="H839" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I839" t="inlineStr">
@@ -37660,7 +37660,7 @@
       <c r="G841" t="inlineStr"/>
       <c r="H841" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I841" t="inlineStr">
@@ -37744,7 +37744,7 @@
       <c r="G843" t="inlineStr"/>
       <c r="H843" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I843" t="inlineStr">
@@ -37828,7 +37828,7 @@
       <c r="G845" t="inlineStr"/>
       <c r="H845" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I845" t="inlineStr">
@@ -37870,7 +37870,7 @@
       <c r="G846" t="inlineStr"/>
       <c r="H846" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I846" t="inlineStr">
@@ -37912,7 +37912,7 @@
       <c r="G847" t="inlineStr"/>
       <c r="H847" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I847" t="inlineStr">
@@ -38100,7 +38100,7 @@
       <c r="G851" t="inlineStr"/>
       <c r="H851" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I851" t="inlineStr">
@@ -38142,7 +38142,7 @@
       <c r="G852" t="inlineStr"/>
       <c r="H852" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I852" t="inlineStr">
@@ -38232,7 +38232,7 @@
       <c r="G854" t="inlineStr"/>
       <c r="H854" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I854" t="inlineStr">
@@ -38378,7 +38378,7 @@
       <c r="G857" t="inlineStr"/>
       <c r="H857" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I857" t="inlineStr">
@@ -38602,7 +38602,7 @@
       <c r="G862" t="inlineStr"/>
       <c r="H862" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I862" t="inlineStr">
@@ -38644,7 +38644,7 @@
       <c r="G863" t="inlineStr"/>
       <c r="H863" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I863" t="inlineStr">
@@ -38686,7 +38686,7 @@
       <c r="G864" t="inlineStr"/>
       <c r="H864" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I864" t="inlineStr">
@@ -38776,7 +38776,7 @@
       <c r="G866" t="inlineStr"/>
       <c r="H866" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I866" t="inlineStr">
@@ -38916,7 +38916,7 @@
       <c r="G869" t="inlineStr"/>
       <c r="H869" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I869" t="inlineStr">
@@ -38958,7 +38958,7 @@
       <c r="G870" t="inlineStr"/>
       <c r="H870" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I870" t="inlineStr">
@@ -39084,7 +39084,7 @@
       <c r="G873" t="inlineStr"/>
       <c r="H873" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I873" t="inlineStr">
@@ -39210,7 +39210,7 @@
       <c r="G876" t="inlineStr"/>
       <c r="H876" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I876" t="inlineStr">
@@ -39342,7 +39342,7 @@
       <c r="G879" t="inlineStr"/>
       <c r="H879" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I879" t="inlineStr">
@@ -39480,7 +39480,7 @@
       <c r="G882" t="inlineStr"/>
       <c r="H882" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I882" t="inlineStr">
@@ -39570,7 +39570,7 @@
       <c r="G884" t="inlineStr"/>
       <c r="H884" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I884" t="inlineStr">
@@ -39660,7 +39660,7 @@
       <c r="G886" t="inlineStr"/>
       <c r="H886" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I886" t="inlineStr">
@@ -39786,7 +39786,7 @@
       <c r="G889" t="inlineStr"/>
       <c r="H889" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I889" t="inlineStr">
@@ -40012,7 +40012,7 @@
       <c r="G894" t="inlineStr"/>
       <c r="H894" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I894" t="inlineStr">
@@ -40054,7 +40054,7 @@
       <c r="G895" t="inlineStr"/>
       <c r="H895" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I895" t="inlineStr">
@@ -40096,7 +40096,7 @@
       <c r="G896" t="inlineStr"/>
       <c r="H896" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I896" t="inlineStr">
@@ -40362,7 +40362,7 @@
       <c r="G902" t="inlineStr"/>
       <c r="H902" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I902" t="inlineStr">
@@ -40488,7 +40488,7 @@
       <c r="G905" t="inlineStr"/>
       <c r="H905" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I905" t="inlineStr">
@@ -40620,7 +40620,7 @@
       <c r="G908" t="inlineStr"/>
       <c r="H908" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I908" t="inlineStr">
@@ -40710,7 +40710,7 @@
       <c r="G910" t="inlineStr"/>
       <c r="H910" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I910" t="inlineStr">
@@ -40800,7 +40800,7 @@
       <c r="G912" t="inlineStr"/>
       <c r="H912" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I912" t="inlineStr">
@@ -40842,7 +40842,7 @@
       <c r="G913" t="inlineStr"/>
       <c r="H913" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I913" t="inlineStr">
@@ -40932,7 +40932,7 @@
       <c r="G915" t="inlineStr"/>
       <c r="H915" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I915" t="inlineStr">
@@ -41064,7 +41064,7 @@
       <c r="G918" t="inlineStr"/>
       <c r="H918" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I918" t="inlineStr">
@@ -41252,7 +41252,7 @@
       <c r="G922" t="inlineStr"/>
       <c r="H922" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I922" t="inlineStr">
@@ -41294,7 +41294,7 @@
       <c r="G923" t="inlineStr"/>
       <c r="H923" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I923" t="inlineStr">
@@ -41426,7 +41426,7 @@
       <c r="G926" t="inlineStr"/>
       <c r="H926" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I926" t="inlineStr">
@@ -41468,7 +41468,7 @@
       <c r="G927" t="inlineStr"/>
       <c r="H927" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I927" t="inlineStr">
@@ -41644,7 +41644,7 @@
       <c r="G931" t="inlineStr"/>
       <c r="H931" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I931" t="inlineStr">
@@ -41776,7 +41776,7 @@
       <c r="G934" t="inlineStr"/>
       <c r="H934" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I934" t="inlineStr">
@@ -41914,7 +41914,7 @@
       <c r="G937" t="inlineStr"/>
       <c r="H937" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I937" t="inlineStr">
@@ -41998,7 +41998,7 @@
       <c r="G939" t="inlineStr"/>
       <c r="H939" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I939" t="inlineStr">
@@ -42192,7 +42192,7 @@
       <c r="G943" t="inlineStr"/>
       <c r="H943" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I943" t="inlineStr">
@@ -42324,7 +42324,7 @@
       <c r="G946" t="inlineStr"/>
       <c r="H946" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I946" t="inlineStr">
@@ -42414,7 +42414,7 @@
       <c r="G948" t="inlineStr"/>
       <c r="H948" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I948" t="inlineStr">
@@ -42642,7 +42642,7 @@
       <c r="G953" t="inlineStr"/>
       <c r="H953" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I953" t="inlineStr">
@@ -42836,7 +42836,7 @@
       <c r="G957" t="inlineStr"/>
       <c r="H957" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I957" t="inlineStr">
@@ -42974,7 +42974,7 @@
       <c r="G960" t="inlineStr"/>
       <c r="H960" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I960" t="inlineStr">
@@ -43216,7 +43216,7 @@
       <c r="G965" t="inlineStr"/>
       <c r="H965" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I965" t="inlineStr">
@@ -43354,7 +43354,7 @@
       <c r="G968" t="inlineStr"/>
       <c r="H968" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I968" t="inlineStr">
@@ -43396,7 +43396,7 @@
       <c r="G969" t="inlineStr"/>
       <c r="H969" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I969" t="inlineStr">
@@ -43534,7 +43534,7 @@
       <c r="G972" t="inlineStr"/>
       <c r="H972" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I972" t="inlineStr">
@@ -43720,7 +43720,7 @@
       <c r="G976" t="inlineStr"/>
       <c r="H976" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I976" t="inlineStr">
@@ -44004,7 +44004,7 @@
       <c r="G982" t="inlineStr"/>
       <c r="H982" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I982" t="inlineStr">
@@ -44184,7 +44184,7 @@
       <c r="G986" t="inlineStr"/>
       <c r="H986" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I986" t="inlineStr">
@@ -44364,7 +44364,7 @@
       <c r="G990" t="inlineStr"/>
       <c r="H990" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I990" t="inlineStr">
@@ -44630,7 +44630,7 @@
       <c r="G996" t="inlineStr"/>
       <c r="H996" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I996" t="inlineStr">
@@ -44818,7 +44818,7 @@
       <c r="G1000" t="inlineStr"/>
       <c r="H1000" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1000" t="inlineStr">
@@ -45172,7 +45172,7 @@
       <c r="G1008" t="inlineStr"/>
       <c r="H1008" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1008" t="inlineStr">
@@ -45556,7 +45556,7 @@
       <c r="G1017" t="inlineStr"/>
       <c r="H1017" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1017" t="inlineStr">
@@ -45862,7 +45862,7 @@
       <c r="G1024" t="inlineStr"/>
       <c r="H1024" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1024" t="inlineStr">
@@ -46072,7 +46072,7 @@
       <c r="G1029" t="inlineStr"/>
       <c r="H1029" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1029" t="inlineStr">
@@ -46300,7 +46300,7 @@
       <c r="G1034" t="inlineStr"/>
       <c r="H1034" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1034" t="inlineStr">
@@ -46476,7 +46476,7 @@
       <c r="G1038" t="inlineStr"/>
       <c r="H1038" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1038" t="inlineStr">
@@ -46614,7 +46614,7 @@
       <c r="G1041" t="inlineStr"/>
       <c r="H1041" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1041" t="inlineStr">
@@ -46754,7 +46754,7 @@
       <c r="G1044" t="inlineStr"/>
       <c r="H1044" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1044" t="inlineStr">
@@ -46948,7 +46948,7 @@
       <c r="G1048" t="inlineStr"/>
       <c r="H1048" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1048" t="inlineStr">
@@ -47094,7 +47094,7 @@
       <c r="G1051" t="inlineStr"/>
       <c r="H1051" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1051" t="inlineStr">
@@ -47234,7 +47234,7 @@
       <c r="G1054" t="inlineStr"/>
       <c r="H1054" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1054" t="inlineStr">
@@ -47276,7 +47276,7 @@
       <c r="G1055" t="inlineStr"/>
       <c r="H1055" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1055" t="inlineStr">
@@ -47366,7 +47366,7 @@
       <c r="G1057" t="inlineStr"/>
       <c r="H1057" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1057" t="inlineStr">
@@ -47542,7 +47542,7 @@
       <c r="G1061" t="inlineStr"/>
       <c r="H1061" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1061" t="inlineStr">
@@ -47584,7 +47584,7 @@
       <c r="G1062" t="inlineStr"/>
       <c r="H1062" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1062" t="inlineStr">
@@ -47802,7 +47802,7 @@
       <c r="G1067" t="inlineStr"/>
       <c r="H1067" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1067" t="inlineStr">
@@ -47844,7 +47844,7 @@
       <c r="G1068" t="inlineStr"/>
       <c r="H1068" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1068" t="inlineStr">
@@ -48080,7 +48080,7 @@
       <c r="G1073" t="inlineStr"/>
       <c r="H1073" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1073" t="inlineStr">
@@ -48324,7 +48324,7 @@
       <c r="G1078" t="inlineStr"/>
       <c r="H1078" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1078" t="inlineStr">
@@ -48554,7 +48554,7 @@
       <c r="G1083" t="inlineStr"/>
       <c r="H1083" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1083" t="inlineStr">
@@ -48840,7 +48840,7 @@
       <c r="G1089" t="inlineStr"/>
       <c r="H1089" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1089" t="inlineStr">
@@ -48882,7 +48882,7 @@
       <c r="G1090" t="inlineStr"/>
       <c r="H1090" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1090" t="inlineStr">
@@ -49022,7 +49022,7 @@
       <c r="G1093" t="inlineStr"/>
       <c r="H1093" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1093" t="inlineStr">
@@ -49064,7 +49064,7 @@
       <c r="G1094" t="inlineStr"/>
       <c r="H1094" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1094" t="inlineStr">
@@ -49106,7 +49106,7 @@
       <c r="G1095" t="inlineStr"/>
       <c r="H1095" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1095" t="inlineStr">
@@ -49148,7 +49148,7 @@
       <c r="G1096" t="inlineStr"/>
       <c r="H1096" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1096" t="inlineStr">
@@ -49286,7 +49286,7 @@
       <c r="G1099" t="inlineStr"/>
       <c r="H1099" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1099" t="inlineStr">
@@ -49466,7 +49466,7 @@
       <c r="G1103" t="inlineStr"/>
       <c r="H1103" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1103" t="inlineStr">
@@ -49646,7 +49646,7 @@
       <c r="G1107" t="inlineStr"/>
       <c r="H1107" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1107" t="inlineStr">
@@ -49778,7 +49778,7 @@
       <c r="G1110" t="inlineStr"/>
       <c r="H1110" t="inlineStr">
         <is>
-          <t>SideRoad,Left</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1110" t="inlineStr">
@@ -49820,7 +49820,7 @@
       <c r="G1111" t="inlineStr"/>
       <c r="H1111" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1111" t="inlineStr">
@@ -50056,7 +50056,7 @@
       <c r="G1116" t="inlineStr"/>
       <c r="H1116" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1116" t="inlineStr">
@@ -50250,7 +50250,7 @@
       <c r="G1120" t="inlineStr"/>
       <c r="H1120" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1120" t="inlineStr">
@@ -50340,7 +50340,7 @@
       <c r="G1122" t="inlineStr"/>
       <c r="H1122" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1122" t="inlineStr">
@@ -50624,7 +50624,7 @@
       <c r="G1128" t="inlineStr"/>
       <c r="H1128" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1128" t="inlineStr">
@@ -50950,7 +50950,7 @@
       <c r="G1135" t="inlineStr"/>
       <c r="H1135" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1135" t="inlineStr">
@@ -51232,7 +51232,7 @@
       <c r="G1141" t="inlineStr"/>
       <c r="H1141" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1141" t="inlineStr">
@@ -51420,7 +51420,7 @@
       <c r="G1145" t="inlineStr"/>
       <c r="H1145" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1145" t="inlineStr">
@@ -51614,7 +51614,7 @@
       <c r="G1149" t="inlineStr"/>
       <c r="H1149" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1149" t="inlineStr">
@@ -51946,7 +51946,7 @@
       <c r="G1156" t="inlineStr"/>
       <c r="H1156" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1156" t="inlineStr">
@@ -52230,7 +52230,7 @@
       <c r="G1162" t="inlineStr"/>
       <c r="H1162" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1162" t="inlineStr">
@@ -52368,7 +52368,7 @@
       <c r="G1165" t="inlineStr"/>
       <c r="H1165" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1165" t="inlineStr">
@@ -52674,7 +52674,7 @@
       <c r="G1172" t="inlineStr"/>
       <c r="H1172" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1172" t="inlineStr">
@@ -52908,7 +52908,7 @@
       <c r="G1177" t="inlineStr"/>
       <c r="H1177" t="inlineStr">
         <is>
-          <t>SideRoad,Right</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1177" t="inlineStr">
@@ -53042,7 +53042,7 @@
       <c r="G1180" t="inlineStr"/>
       <c r="H1180" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1180" t="inlineStr">
@@ -53264,7 +53264,7 @@
       <c r="G1185" t="inlineStr"/>
       <c r="H1185" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1185" t="inlineStr">
@@ -53534,7 +53534,7 @@
       <c r="G1191" t="inlineStr"/>
       <c r="H1191" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1191" t="inlineStr">
@@ -53800,7 +53800,7 @@
       <c r="G1197" t="inlineStr"/>
       <c r="H1197" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1197" t="inlineStr">
@@ -53980,7 +53980,7 @@
       <c r="G1201" t="inlineStr"/>
       <c r="H1201" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1201" t="inlineStr">
@@ -54250,7 +54250,7 @@
       <c r="G1207" t="inlineStr"/>
       <c r="H1207" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1207" t="inlineStr">
@@ -54472,7 +54472,7 @@
       <c r="G1212" t="inlineStr"/>
       <c r="H1212" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1212" t="inlineStr">
@@ -54738,7 +54738,7 @@
       <c r="G1218" t="inlineStr"/>
       <c r="H1218" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1218" t="inlineStr">
@@ -54920,7 +54920,7 @@
       <c r="G1222" t="inlineStr"/>
       <c r="H1222" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1222" t="inlineStr">
@@ -55136,7 +55136,7 @@
       <c r="G1227" t="inlineStr"/>
       <c r="H1227" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1227" t="inlineStr">
@@ -55324,7 +55324,7 @@
       <c r="G1231" t="inlineStr"/>
       <c r="H1231" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1231" t="inlineStr">
@@ -55510,7 +55510,7 @@
       <c r="G1235" t="inlineStr"/>
       <c r="H1235" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1235" t="inlineStr">
@@ -55656,7 +55656,7 @@
       <c r="G1238" t="inlineStr"/>
       <c r="H1238" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1238" t="inlineStr">
@@ -55794,7 +55794,7 @@
       <c r="G1241" t="inlineStr"/>
       <c r="H1241" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1241" t="inlineStr">
@@ -55980,7 +55980,7 @@
       <c r="G1245" t="inlineStr"/>
       <c r="H1245" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1245" t="inlineStr">
@@ -56168,7 +56168,7 @@
       <c r="G1249" t="inlineStr"/>
       <c r="H1249" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1249" t="inlineStr">
@@ -56258,7 +56258,7 @@
       <c r="G1251" t="inlineStr"/>
       <c r="H1251" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1251" t="inlineStr">
@@ -56398,7 +56398,7 @@
       <c r="G1254" t="inlineStr"/>
       <c r="H1254" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1254" t="inlineStr">
@@ -56488,7 +56488,7 @@
       <c r="G1256" t="inlineStr"/>
       <c r="H1256" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1256" t="inlineStr">
@@ -56780,7 +56780,7 @@
       <c r="G1262" t="inlineStr"/>
       <c r="H1262" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1262" t="inlineStr">
@@ -57038,7 +57038,7 @@
       <c r="G1268" t="inlineStr"/>
       <c r="H1268" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1268" t="inlineStr">
@@ -57268,7 +57268,7 @@
       <c r="G1273" t="inlineStr"/>
       <c r="H1273" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1273" t="inlineStr">
@@ -57450,7 +57450,7 @@
       <c r="G1277" t="inlineStr"/>
       <c r="H1277" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1277" t="inlineStr">
@@ -57770,7 +57770,7 @@
       <c r="G1284" t="inlineStr"/>
       <c r="H1284" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1284" t="inlineStr">
@@ -58038,7 +58038,7 @@
       <c r="G1290" t="inlineStr"/>
       <c r="H1290" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1290" t="inlineStr">
@@ -58340,7 +58340,7 @@
       <c r="G1297" t="inlineStr"/>
       <c r="H1297" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1297" t="inlineStr">
@@ -58558,7 +58558,7 @@
       <c r="G1302" t="inlineStr"/>
       <c r="H1302" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1302" t="inlineStr">
@@ -58952,7 +58952,7 @@
       <c r="G1311" t="inlineStr"/>
       <c r="H1311" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1311" t="inlineStr">
@@ -59472,7 +59472,7 @@
       <c r="G1323" t="inlineStr"/>
       <c r="H1323" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1323" t="inlineStr">
@@ -59606,7 +59606,7 @@
       <c r="G1326" t="inlineStr"/>
       <c r="H1326" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1326" t="inlineStr">
@@ -59740,7 +59740,7 @@
       <c r="G1329" t="inlineStr"/>
       <c r="H1329" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1329" t="inlineStr">
@@ -59866,7 +59866,7 @@
       <c r="G1332" t="inlineStr"/>
       <c r="H1332" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1332" t="inlineStr">
@@ -60000,7 +60000,7 @@
       <c r="G1335" t="inlineStr"/>
       <c r="H1335" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1335" t="inlineStr">
@@ -60176,7 +60176,7 @@
       <c r="G1339" t="inlineStr"/>
       <c r="H1339" t="inlineStr">
         <is>
-          <t>KmPost</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1339" t="inlineStr">
@@ -60218,7 +60218,7 @@
       <c r="G1340" t="inlineStr"/>
       <c r="H1340" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1340" t="inlineStr">

</xml_diff>

<commit_message>
Merge of all commits
</commit_message>
<xml_diff>
--- a/EPA1352-G11-A2/check_N1_df.xlsx
+++ b/EPA1352-G11-A2/check_N1_df.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>model_type</t>
+          <t>type</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -516,7 +516,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>source</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -600,7 +600,7 @@
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -642,7 +642,7 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -684,7 +684,7 @@
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -768,7 +768,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -810,7 +810,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -852,7 +852,7 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -894,7 +894,7 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -936,7 +936,7 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -978,7 +978,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1020,7 +1020,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1062,7 +1062,7 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1202,7 +1202,7 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1244,7 +1244,7 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1286,7 +1286,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1472,7 +1472,7 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1604,7 +1604,7 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1750,7 +1750,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -1792,7 +1792,7 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -1882,7 +1882,7 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -1924,7 +1924,7 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2008,7 +2008,7 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2050,7 +2050,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2184,7 +2184,7 @@
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2416,7 +2416,7 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
@@ -2562,7 +2562,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -2700,7 +2700,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -2742,7 +2742,7 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -2882,7 +2882,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -2966,7 +2966,7 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3198,7 +3198,7 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
@@ -3288,7 +3288,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3378,7 +3378,7 @@
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -3420,7 +3420,7 @@
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -3558,7 +3558,7 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -3648,7 +3648,7 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3836,7 +3836,7 @@
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3982,7 +3982,7 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -4214,7 +4214,7 @@
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4256,7 +4256,7 @@
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -4390,7 +4390,7 @@
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4480,7 +4480,7 @@
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -4668,7 +4668,7 @@
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -4710,7 +4710,7 @@
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
@@ -4892,7 +4892,7 @@
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -4982,7 +4982,7 @@
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -5024,7 +5024,7 @@
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -5108,7 +5108,7 @@
       <c r="G104" t="inlineStr"/>
       <c r="H104" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -5150,7 +5150,7 @@
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -5284,7 +5284,7 @@
       <c r="G108" t="inlineStr"/>
       <c r="H108" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
@@ -5368,7 +5368,7 @@
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I110" t="inlineStr">
@@ -5410,7 +5410,7 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
@@ -5452,7 +5452,7 @@
       <c r="G112" t="inlineStr"/>
       <c r="H112" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I112" t="inlineStr">
@@ -5586,7 +5586,7 @@
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -5628,7 +5628,7 @@
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -5670,7 +5670,7 @@
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -5754,7 +5754,7 @@
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I119" t="inlineStr">
@@ -5796,7 +5796,7 @@
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -5838,7 +5838,7 @@
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -5922,7 +5922,7 @@
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
@@ -5964,7 +5964,7 @@
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -6006,7 +6006,7 @@
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I125" t="inlineStr">
@@ -6140,7 +6140,7 @@
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -6182,7 +6182,7 @@
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -6316,7 +6316,7 @@
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
@@ -6358,7 +6358,7 @@
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I133" t="inlineStr">
@@ -6442,7 +6442,7 @@
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -6484,7 +6484,7 @@
       <c r="G136" t="inlineStr"/>
       <c r="H136" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -6526,7 +6526,7 @@
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -6568,7 +6568,7 @@
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -6708,7 +6708,7 @@
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
@@ -6750,7 +6750,7 @@
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -6792,7 +6792,7 @@
       <c r="G143" t="inlineStr"/>
       <c r="H143" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
@@ -6876,7 +6876,7 @@
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
@@ -6918,7 +6918,7 @@
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -7002,7 +7002,7 @@
       <c r="G148" t="inlineStr"/>
       <c r="H148" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
@@ -7044,7 +7044,7 @@
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
@@ -7086,7 +7086,7 @@
       <c r="G150" t="inlineStr"/>
       <c r="H150" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I150" t="inlineStr">
@@ -7128,7 +7128,7 @@
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
@@ -7254,7 +7254,7 @@
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
@@ -7296,7 +7296,7 @@
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I155" t="inlineStr">
@@ -7338,7 +7338,7 @@
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
@@ -7422,7 +7422,7 @@
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
@@ -7464,7 +7464,7 @@
       <c r="G159" t="inlineStr"/>
       <c r="H159" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I159" t="inlineStr">
@@ -7554,7 +7554,7 @@
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I161" t="inlineStr">
@@ -7596,7 +7596,7 @@
       <c r="G162" t="inlineStr"/>
       <c r="H162" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
@@ -7638,7 +7638,7 @@
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -7680,7 +7680,7 @@
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I164" t="inlineStr">
@@ -7722,7 +7722,7 @@
       <c r="G165" t="inlineStr"/>
       <c r="H165" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I165" t="inlineStr">
@@ -7764,7 +7764,7 @@
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I166" t="inlineStr">
@@ -7904,7 +7904,7 @@
       <c r="G169" t="inlineStr"/>
       <c r="H169" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I169" t="inlineStr">
@@ -7946,7 +7946,7 @@
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I170" t="inlineStr">
@@ -7988,7 +7988,7 @@
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I171" t="inlineStr">
@@ -8078,7 +8078,7 @@
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I173" t="inlineStr">
@@ -8168,7 +8168,7 @@
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
@@ -8210,7 +8210,7 @@
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
@@ -8252,7 +8252,7 @@
       <c r="G177" t="inlineStr"/>
       <c r="H177" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I177" t="inlineStr">
@@ -8294,7 +8294,7 @@
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
@@ -8384,7 +8384,7 @@
       <c r="G180" t="inlineStr"/>
       <c r="H180" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
@@ -8426,7 +8426,7 @@
       <c r="G181" t="inlineStr"/>
       <c r="H181" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I181" t="inlineStr">
@@ -8468,7 +8468,7 @@
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I182" t="inlineStr">
@@ -8552,7 +8552,7 @@
       <c r="G184" t="inlineStr"/>
       <c r="H184" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I184" t="inlineStr">
@@ -8642,7 +8642,7 @@
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I186" t="inlineStr">
@@ -8684,7 +8684,7 @@
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
@@ -8768,7 +8768,7 @@
       <c r="G189" t="inlineStr"/>
       <c r="H189" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I189" t="inlineStr">
@@ -8810,7 +8810,7 @@
       <c r="G190" t="inlineStr"/>
       <c r="H190" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
@@ -8852,7 +8852,7 @@
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I191" t="inlineStr">
@@ -8894,7 +8894,7 @@
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I192" t="inlineStr">
@@ -8936,7 +8936,7 @@
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I193" t="inlineStr">
@@ -8978,7 +8978,7 @@
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
@@ -9112,7 +9112,7 @@
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I197" t="inlineStr">
@@ -9154,7 +9154,7 @@
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I198" t="inlineStr">
@@ -9196,7 +9196,7 @@
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I199" t="inlineStr">
@@ -9238,7 +9238,7 @@
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I200" t="inlineStr">
@@ -9280,7 +9280,7 @@
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I201" t="inlineStr">
@@ -9414,7 +9414,7 @@
       <c r="G204" t="inlineStr"/>
       <c r="H204" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I204" t="inlineStr">
@@ -9456,7 +9456,7 @@
       <c r="G205" t="inlineStr"/>
       <c r="H205" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I205" t="inlineStr">
@@ -9498,7 +9498,7 @@
       <c r="G206" t="inlineStr"/>
       <c r="H206" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
@@ -9540,7 +9540,7 @@
       <c r="G207" t="inlineStr"/>
       <c r="H207" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I207" t="inlineStr">
@@ -9674,7 +9674,7 @@
       <c r="G210" t="inlineStr"/>
       <c r="H210" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
@@ -9716,7 +9716,7 @@
       <c r="G211" t="inlineStr"/>
       <c r="H211" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
@@ -9758,7 +9758,7 @@
       <c r="G212" t="inlineStr"/>
       <c r="H212" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
@@ -9848,7 +9848,7 @@
       <c r="G214" t="inlineStr"/>
       <c r="H214" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
@@ -9982,7 +9982,7 @@
       <c r="G217" t="inlineStr"/>
       <c r="H217" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I217" t="inlineStr">
@@ -10024,7 +10024,7 @@
       <c r="G218" t="inlineStr"/>
       <c r="H218" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I218" t="inlineStr">
@@ -10198,7 +10198,7 @@
       <c r="G222" t="inlineStr"/>
       <c r="H222" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I222" t="inlineStr">
@@ -10332,7 +10332,7 @@
       <c r="G225" t="inlineStr"/>
       <c r="H225" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
@@ -10374,7 +10374,7 @@
       <c r="G226" t="inlineStr"/>
       <c r="H226" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
@@ -10464,7 +10464,7 @@
       <c r="G228" t="inlineStr"/>
       <c r="H228" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
@@ -10604,7 +10604,7 @@
       <c r="G231" t="inlineStr"/>
       <c r="H231" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I231" t="inlineStr">
@@ -10688,7 +10688,7 @@
       <c r="G233" t="inlineStr"/>
       <c r="H233" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
@@ -10730,7 +10730,7 @@
       <c r="G234" t="inlineStr"/>
       <c r="H234" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
@@ -10864,7 +10864,7 @@
       <c r="G237" t="inlineStr"/>
       <c r="H237" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
@@ -10906,7 +10906,7 @@
       <c r="G238" t="inlineStr"/>
       <c r="H238" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
@@ -10948,7 +10948,7 @@
       <c r="G239" t="inlineStr"/>
       <c r="H239" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
@@ -11088,7 +11088,7 @@
       <c r="G242" t="inlineStr"/>
       <c r="H242" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I242" t="inlineStr">
@@ -11270,7 +11270,7 @@
       <c r="G246" t="inlineStr"/>
       <c r="H246" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
@@ -11360,7 +11360,7 @@
       <c r="G248" t="inlineStr"/>
       <c r="H248" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
@@ -11500,7 +11500,7 @@
       <c r="G251" t="inlineStr"/>
       <c r="H251" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
@@ -11590,7 +11590,7 @@
       <c r="G253" t="inlineStr"/>
       <c r="H253" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
@@ -11674,7 +11674,7 @@
       <c r="G255" t="inlineStr"/>
       <c r="H255" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
@@ -11716,7 +11716,7 @@
       <c r="G256" t="inlineStr"/>
       <c r="H256" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -11890,7 +11890,7 @@
       <c r="G260" t="inlineStr"/>
       <c r="H260" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
@@ -11980,7 +11980,7 @@
       <c r="G262" t="inlineStr"/>
       <c r="H262" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
@@ -12210,7 +12210,7 @@
       <c r="G267" t="inlineStr"/>
       <c r="H267" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I267" t="inlineStr">
@@ -12348,7 +12348,7 @@
       <c r="G270" t="inlineStr"/>
       <c r="H270" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I270" t="inlineStr">
@@ -12480,7 +12480,7 @@
       <c r="G273" t="inlineStr"/>
       <c r="H273" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I273" t="inlineStr">
@@ -12522,7 +12522,7 @@
       <c r="G274" t="inlineStr"/>
       <c r="H274" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
@@ -12606,7 +12606,7 @@
       <c r="G276" t="inlineStr"/>
       <c r="H276" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I276" t="inlineStr">
@@ -12696,7 +12696,7 @@
       <c r="G278" t="inlineStr"/>
       <c r="H278" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I278" t="inlineStr">
@@ -12786,7 +12786,7 @@
       <c r="G280" t="inlineStr"/>
       <c r="H280" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I280" t="inlineStr">
@@ -12876,7 +12876,7 @@
       <c r="G282" t="inlineStr"/>
       <c r="H282" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I282" t="inlineStr">
@@ -13016,7 +13016,7 @@
       <c r="G285" t="inlineStr"/>
       <c r="H285" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I285" t="inlineStr">
@@ -13106,7 +13106,7 @@
       <c r="G287" t="inlineStr"/>
       <c r="H287" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I287" t="inlineStr">
@@ -13246,7 +13246,7 @@
       <c r="G290" t="inlineStr"/>
       <c r="H290" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I290" t="inlineStr">
@@ -13336,7 +13336,7 @@
       <c r="G292" t="inlineStr"/>
       <c r="H292" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I292" t="inlineStr">
@@ -13378,7 +13378,7 @@
       <c r="G293" t="inlineStr"/>
       <c r="H293" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I293" t="inlineStr">
@@ -13462,7 +13462,7 @@
       <c r="G295" t="inlineStr"/>
       <c r="H295" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I295" t="inlineStr">
@@ -13552,7 +13552,7 @@
       <c r="G297" t="inlineStr"/>
       <c r="H297" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I297" t="inlineStr">
@@ -13642,7 +13642,7 @@
       <c r="G299" t="inlineStr"/>
       <c r="H299" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I299" t="inlineStr">
@@ -13774,7 +13774,7 @@
       <c r="G302" t="inlineStr"/>
       <c r="H302" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I302" t="inlineStr">
@@ -13864,7 +13864,7 @@
       <c r="G304" t="inlineStr"/>
       <c r="H304" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I304" t="inlineStr">
@@ -13906,7 +13906,7 @@
       <c r="G305" t="inlineStr"/>
       <c r="H305" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I305" t="inlineStr">
@@ -14038,7 +14038,7 @@
       <c r="G308" t="inlineStr"/>
       <c r="H308" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I308" t="inlineStr">
@@ -14176,7 +14176,7 @@
       <c r="G311" t="inlineStr"/>
       <c r="H311" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I311" t="inlineStr">
@@ -14266,7 +14266,7 @@
       <c r="G313" t="inlineStr"/>
       <c r="H313" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I313" t="inlineStr">
@@ -14442,7 +14442,7 @@
       <c r="G317" t="inlineStr"/>
       <c r="H317" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I317" t="inlineStr">
@@ -14532,7 +14532,7 @@
       <c r="G319" t="inlineStr"/>
       <c r="H319" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
@@ -14574,7 +14574,7 @@
       <c r="G320" t="inlineStr"/>
       <c r="H320" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I320" t="inlineStr">
@@ -14658,7 +14658,7 @@
       <c r="G322" t="inlineStr"/>
       <c r="H322" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
@@ -14700,7 +14700,7 @@
       <c r="G323" t="inlineStr"/>
       <c r="H323" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I323" t="inlineStr">
@@ -14742,7 +14742,7 @@
       <c r="G324" t="inlineStr"/>
       <c r="H324" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I324" t="inlineStr">
@@ -14784,7 +14784,7 @@
       <c r="G325" t="inlineStr"/>
       <c r="H325" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I325" t="inlineStr">
@@ -14826,7 +14826,7 @@
       <c r="G326" t="inlineStr"/>
       <c r="H326" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I326" t="inlineStr">
@@ -14910,7 +14910,7 @@
       <c r="G328" t="inlineStr"/>
       <c r="H328" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I328" t="inlineStr">
@@ -14952,7 +14952,7 @@
       <c r="G329" t="inlineStr"/>
       <c r="H329" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I329" t="inlineStr">
@@ -15042,7 +15042,7 @@
       <c r="G331" t="inlineStr"/>
       <c r="H331" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I331" t="inlineStr">
@@ -15084,7 +15084,7 @@
       <c r="G332" t="inlineStr"/>
       <c r="H332" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I332" t="inlineStr">
@@ -15126,7 +15126,7 @@
       <c r="G333" t="inlineStr"/>
       <c r="H333" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I333" t="inlineStr">
@@ -15252,7 +15252,7 @@
       <c r="G336" t="inlineStr"/>
       <c r="H336" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I336" t="inlineStr">
@@ -15294,7 +15294,7 @@
       <c r="G337" t="inlineStr"/>
       <c r="H337" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I337" t="inlineStr">
@@ -15336,7 +15336,7 @@
       <c r="G338" t="inlineStr"/>
       <c r="H338" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I338" t="inlineStr">
@@ -15378,7 +15378,7 @@
       <c r="G339" t="inlineStr"/>
       <c r="H339" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I339" t="inlineStr">
@@ -15512,7 +15512,7 @@
       <c r="G342" t="inlineStr"/>
       <c r="H342" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I342" t="inlineStr">
@@ -15554,7 +15554,7 @@
       <c r="G343" t="inlineStr"/>
       <c r="H343" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I343" t="inlineStr">
@@ -15596,7 +15596,7 @@
       <c r="G344" t="inlineStr"/>
       <c r="H344" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I344" t="inlineStr">
@@ -15638,7 +15638,7 @@
       <c r="G345" t="inlineStr"/>
       <c r="H345" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I345" t="inlineStr">
@@ -15680,7 +15680,7 @@
       <c r="G346" t="inlineStr"/>
       <c r="H346" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I346" t="inlineStr">
@@ -15722,7 +15722,7 @@
       <c r="G347" t="inlineStr"/>
       <c r="H347" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I347" t="inlineStr">
@@ -15764,7 +15764,7 @@
       <c r="G348" t="inlineStr"/>
       <c r="H348" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I348" t="inlineStr">
@@ -15898,7 +15898,7 @@
       <c r="G351" t="inlineStr"/>
       <c r="H351" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I351" t="inlineStr">
@@ -15940,7 +15940,7 @@
       <c r="G352" t="inlineStr"/>
       <c r="H352" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I352" t="inlineStr">
@@ -15982,7 +15982,7 @@
       <c r="G353" t="inlineStr"/>
       <c r="H353" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I353" t="inlineStr">
@@ -16024,7 +16024,7 @@
       <c r="G354" t="inlineStr"/>
       <c r="H354" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I354" t="inlineStr">
@@ -16066,7 +16066,7 @@
       <c r="G355" t="inlineStr"/>
       <c r="H355" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I355" t="inlineStr">
@@ -16108,7 +16108,7 @@
       <c r="G356" t="inlineStr"/>
       <c r="H356" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I356" t="inlineStr">
@@ -16150,7 +16150,7 @@
       <c r="G357" t="inlineStr"/>
       <c r="H357" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I357" t="inlineStr">
@@ -16192,7 +16192,7 @@
       <c r="G358" t="inlineStr"/>
       <c r="H358" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I358" t="inlineStr">
@@ -16326,7 +16326,7 @@
       <c r="G361" t="inlineStr"/>
       <c r="H361" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I361" t="inlineStr">
@@ -16368,7 +16368,7 @@
       <c r="G362" t="inlineStr"/>
       <c r="H362" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I362" t="inlineStr">
@@ -16410,7 +16410,7 @@
       <c r="G363" t="inlineStr"/>
       <c r="H363" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I363" t="inlineStr">
@@ -16452,7 +16452,7 @@
       <c r="G364" t="inlineStr"/>
       <c r="H364" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I364" t="inlineStr">
@@ -16494,7 +16494,7 @@
       <c r="G365" t="inlineStr"/>
       <c r="H365" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I365" t="inlineStr">
@@ -16536,7 +16536,7 @@
       <c r="G366" t="inlineStr"/>
       <c r="H366" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I366" t="inlineStr">
@@ -16670,7 +16670,7 @@
       <c r="G369" t="inlineStr"/>
       <c r="H369" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I369" t="inlineStr">
@@ -16760,7 +16760,7 @@
       <c r="G371" t="inlineStr"/>
       <c r="H371" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I371" t="inlineStr">
@@ -16802,7 +16802,7 @@
       <c r="G372" t="inlineStr"/>
       <c r="H372" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I372" t="inlineStr">
@@ -16844,7 +16844,7 @@
       <c r="G373" t="inlineStr"/>
       <c r="H373" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I373" t="inlineStr">
@@ -16886,7 +16886,7 @@
       <c r="G374" t="inlineStr"/>
       <c r="H374" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I374" t="inlineStr">
@@ -16970,7 +16970,7 @@
       <c r="G376" t="inlineStr"/>
       <c r="H376" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I376" t="inlineStr">
@@ -17108,7 +17108,7 @@
       <c r="G379" t="inlineStr"/>
       <c r="H379" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I379" t="inlineStr">
@@ -17246,7 +17246,7 @@
       <c r="G382" t="inlineStr"/>
       <c r="H382" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I382" t="inlineStr">
@@ -17384,7 +17384,7 @@
       <c r="G385" t="inlineStr"/>
       <c r="H385" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I385" t="inlineStr">
@@ -17522,7 +17522,7 @@
       <c r="G388" t="inlineStr"/>
       <c r="H388" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I388" t="inlineStr">
@@ -17752,7 +17752,7 @@
       <c r="G393" t="inlineStr"/>
       <c r="H393" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I393" t="inlineStr">
@@ -17836,7 +17836,7 @@
       <c r="G395" t="inlineStr"/>
       <c r="H395" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I395" t="inlineStr">
@@ -17920,7 +17920,7 @@
       <c r="G397" t="inlineStr"/>
       <c r="H397" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I397" t="inlineStr">
@@ -17962,7 +17962,7 @@
       <c r="G398" t="inlineStr"/>
       <c r="H398" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I398" t="inlineStr">
@@ -18130,7 +18130,7 @@
       <c r="G402" t="inlineStr"/>
       <c r="H402" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I402" t="inlineStr">
@@ -18220,7 +18220,7 @@
       <c r="G404" t="inlineStr"/>
       <c r="H404" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I404" t="inlineStr">
@@ -18352,7 +18352,7 @@
       <c r="G407" t="inlineStr"/>
       <c r="H407" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I407" t="inlineStr">
@@ -18436,7 +18436,7 @@
       <c r="G409" t="inlineStr"/>
       <c r="H409" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I409" t="inlineStr">
@@ -18526,7 +18526,7 @@
       <c r="G411" t="inlineStr"/>
       <c r="H411" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I411" t="inlineStr">
@@ -18610,7 +18610,7 @@
       <c r="G413" t="inlineStr"/>
       <c r="H413" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I413" t="inlineStr">
@@ -18742,7 +18742,7 @@
       <c r="G416" t="inlineStr"/>
       <c r="H416" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I416" t="inlineStr">
@@ -18832,7 +18832,7 @@
       <c r="G418" t="inlineStr"/>
       <c r="H418" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I418" t="inlineStr">
@@ -18978,7 +18978,7 @@
       <c r="G421" t="inlineStr"/>
       <c r="H421" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I421" t="inlineStr">
@@ -19062,7 +19062,7 @@
       <c r="G423" t="inlineStr"/>
       <c r="H423" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I423" t="inlineStr">
@@ -19146,7 +19146,7 @@
       <c r="G425" t="inlineStr"/>
       <c r="H425" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I425" t="inlineStr">
@@ -19236,7 +19236,7 @@
       <c r="G427" t="inlineStr"/>
       <c r="H427" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I427" t="inlineStr">
@@ -19326,7 +19326,7 @@
       <c r="G429" t="inlineStr"/>
       <c r="H429" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I429" t="inlineStr">
@@ -19452,7 +19452,7 @@
       <c r="G432" t="inlineStr"/>
       <c r="H432" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I432" t="inlineStr">
@@ -19584,7 +19584,7 @@
       <c r="G435" t="inlineStr"/>
       <c r="H435" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I435" t="inlineStr">
@@ -19758,7 +19758,7 @@
       <c r="G439" t="inlineStr"/>
       <c r="H439" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I439" t="inlineStr">
@@ -19848,7 +19848,7 @@
       <c r="G441" t="inlineStr"/>
       <c r="H441" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I441" t="inlineStr">
@@ -19980,7 +19980,7 @@
       <c r="G444" t="inlineStr"/>
       <c r="H444" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I444" t="inlineStr">
@@ -20118,7 +20118,7 @@
       <c r="G447" t="inlineStr"/>
       <c r="H447" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I447" t="inlineStr">
@@ -20160,7 +20160,7 @@
       <c r="G448" t="inlineStr"/>
       <c r="H448" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I448" t="inlineStr">
@@ -20286,7 +20286,7 @@
       <c r="G451" t="inlineStr"/>
       <c r="H451" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I451" t="inlineStr">
@@ -20424,7 +20424,7 @@
       <c r="G454" t="inlineStr"/>
       <c r="H454" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I454" t="inlineStr">
@@ -20550,7 +20550,7 @@
       <c r="G457" t="inlineStr"/>
       <c r="H457" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I457" t="inlineStr">
@@ -20688,7 +20688,7 @@
       <c r="G460" t="inlineStr"/>
       <c r="H460" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I460" t="inlineStr">
@@ -20778,7 +20778,7 @@
       <c r="G462" t="inlineStr"/>
       <c r="H462" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I462" t="inlineStr">
@@ -20916,7 +20916,7 @@
       <c r="G465" t="inlineStr"/>
       <c r="H465" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I465" t="inlineStr">
@@ -21182,7 +21182,7 @@
       <c r="G471" t="inlineStr"/>
       <c r="H471" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I471" t="inlineStr">
@@ -21314,7 +21314,7 @@
       <c r="G474" t="inlineStr"/>
       <c r="H474" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I474" t="inlineStr">
@@ -21404,7 +21404,7 @@
       <c r="G476" t="inlineStr"/>
       <c r="H476" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I476" t="inlineStr">
@@ -21620,7 +21620,7 @@
       <c r="G481" t="inlineStr"/>
       <c r="H481" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I481" t="inlineStr">
@@ -21710,7 +21710,7 @@
       <c r="G483" t="inlineStr"/>
       <c r="H483" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I483" t="inlineStr">
@@ -21850,7 +21850,7 @@
       <c r="G486" t="inlineStr"/>
       <c r="H486" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I486" t="inlineStr">
@@ -21934,7 +21934,7 @@
       <c r="G488" t="inlineStr"/>
       <c r="H488" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I488" t="inlineStr">
@@ -22080,7 +22080,7 @@
       <c r="G491" t="inlineStr"/>
       <c r="H491" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I491" t="inlineStr">
@@ -22304,7 +22304,7 @@
       <c r="G496" t="inlineStr"/>
       <c r="H496" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I496" t="inlineStr">
@@ -22346,7 +22346,7 @@
       <c r="G497" t="inlineStr"/>
       <c r="H497" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I497" t="inlineStr">
@@ -22492,7 +22492,7 @@
       <c r="G500" t="inlineStr"/>
       <c r="H500" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I500" t="inlineStr">
@@ -22582,7 +22582,7 @@
       <c r="G502" t="inlineStr"/>
       <c r="H502" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I502" t="inlineStr">
@@ -22672,7 +22672,7 @@
       <c r="G504" t="inlineStr"/>
       <c r="H504" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I504" t="inlineStr">
@@ -22806,7 +22806,7 @@
       <c r="G507" t="inlineStr"/>
       <c r="H507" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I507" t="inlineStr">
@@ -23080,7 +23080,7 @@
       <c r="G513" t="inlineStr"/>
       <c r="H513" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I513" t="inlineStr">
@@ -23360,7 +23360,7 @@
       <c r="G519" t="inlineStr"/>
       <c r="H519" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I519" t="inlineStr">
@@ -23500,7 +23500,7 @@
       <c r="G522" t="inlineStr"/>
       <c r="H522" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I522" t="inlineStr">
@@ -23590,7 +23590,7 @@
       <c r="G524" t="inlineStr"/>
       <c r="H524" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I524" t="inlineStr">
@@ -23772,7 +23772,7 @@
       <c r="G528" t="inlineStr"/>
       <c r="H528" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I528" t="inlineStr">
@@ -23856,7 +23856,7 @@
       <c r="G530" t="inlineStr"/>
       <c r="H530" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I530" t="inlineStr">
@@ -23898,7 +23898,7 @@
       <c r="G531" t="inlineStr"/>
       <c r="H531" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I531" t="inlineStr">
@@ -24038,7 +24038,7 @@
       <c r="G534" t="inlineStr"/>
       <c r="H534" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I534" t="inlineStr">
@@ -24080,7 +24080,7 @@
       <c r="G535" t="inlineStr"/>
       <c r="H535" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I535" t="inlineStr">
@@ -24226,7 +24226,7 @@
       <c r="G538" t="inlineStr"/>
       <c r="H538" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I538" t="inlineStr">
@@ -24402,7 +24402,7 @@
       <c r="G542" t="inlineStr"/>
       <c r="H542" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I542" t="inlineStr">
@@ -24444,7 +24444,7 @@
       <c r="G543" t="inlineStr"/>
       <c r="H543" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I543" t="inlineStr">
@@ -24578,7 +24578,7 @@
       <c r="G546" t="inlineStr"/>
       <c r="H546" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I546" t="inlineStr">
@@ -24620,7 +24620,7 @@
       <c r="G547" t="inlineStr"/>
       <c r="H547" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I547" t="inlineStr">
@@ -24704,7 +24704,7 @@
       <c r="G549" t="inlineStr"/>
       <c r="H549" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I549" t="inlineStr">
@@ -24746,7 +24746,7 @@
       <c r="G550" t="inlineStr"/>
       <c r="H550" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I550" t="inlineStr">
@@ -24788,7 +24788,7 @@
       <c r="G551" t="inlineStr"/>
       <c r="H551" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I551" t="inlineStr">
@@ -24928,7 +24928,7 @@
       <c r="G554" t="inlineStr"/>
       <c r="H554" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I554" t="inlineStr">
@@ -24970,7 +24970,7 @@
       <c r="G555" t="inlineStr"/>
       <c r="H555" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I555" t="inlineStr">
@@ -25146,7 +25146,7 @@
       <c r="G559" t="inlineStr"/>
       <c r="H559" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I559" t="inlineStr">
@@ -25236,7 +25236,7 @@
       <c r="G561" t="inlineStr"/>
       <c r="H561" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I561" t="inlineStr">
@@ -25376,7 +25376,7 @@
       <c r="G564" t="inlineStr"/>
       <c r="H564" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I564" t="inlineStr">
@@ -25418,7 +25418,7 @@
       <c r="G565" t="inlineStr"/>
       <c r="H565" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I565" t="inlineStr">
@@ -25460,7 +25460,7 @@
       <c r="G566" t="inlineStr"/>
       <c r="H566" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I566" t="inlineStr">
@@ -25502,7 +25502,7 @@
       <c r="G567" t="inlineStr"/>
       <c r="H567" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I567" t="inlineStr">
@@ -25544,7 +25544,7 @@
       <c r="G568" t="inlineStr"/>
       <c r="H568" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I568" t="inlineStr">
@@ -25634,7 +25634,7 @@
       <c r="G570" t="inlineStr"/>
       <c r="H570" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I570" t="inlineStr">
@@ -25780,7 +25780,7 @@
       <c r="G573" t="inlineStr"/>
       <c r="H573" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I573" t="inlineStr">
@@ -25920,7 +25920,7 @@
       <c r="G576" t="inlineStr"/>
       <c r="H576" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I576" t="inlineStr">
@@ -26152,7 +26152,7 @@
       <c r="G581" t="inlineStr"/>
       <c r="H581" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I581" t="inlineStr">
@@ -26242,7 +26242,7 @@
       <c r="G583" t="inlineStr"/>
       <c r="H583" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I583" t="inlineStr">
@@ -26424,7 +26424,7 @@
       <c r="G587" t="inlineStr"/>
       <c r="H587" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I587" t="inlineStr">
@@ -26466,7 +26466,7 @@
       <c r="G588" t="inlineStr"/>
       <c r="H588" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I588" t="inlineStr">
@@ -26508,7 +26508,7 @@
       <c r="G589" t="inlineStr"/>
       <c r="H589" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I589" t="inlineStr">
@@ -26592,7 +26592,7 @@
       <c r="G591" t="inlineStr"/>
       <c r="H591" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I591" t="inlineStr">
@@ -26724,7 +26724,7 @@
       <c r="G594" t="inlineStr"/>
       <c r="H594" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I594" t="inlineStr">
@@ -26814,7 +26814,7 @@
       <c r="G596" t="inlineStr"/>
       <c r="H596" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I596" t="inlineStr">
@@ -26856,7 +26856,7 @@
       <c r="G597" t="inlineStr"/>
       <c r="H597" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I597" t="inlineStr">
@@ -27024,7 +27024,7 @@
       <c r="G601" t="inlineStr"/>
       <c r="H601" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I601" t="inlineStr">
@@ -27156,7 +27156,7 @@
       <c r="G604" t="inlineStr"/>
       <c r="H604" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I604" t="inlineStr">
@@ -27198,7 +27198,7 @@
       <c r="G605" t="inlineStr"/>
       <c r="H605" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I605" t="inlineStr">
@@ -27240,7 +27240,7 @@
       <c r="G606" t="inlineStr"/>
       <c r="H606" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I606" t="inlineStr">
@@ -27330,7 +27330,7 @@
       <c r="G608" t="inlineStr"/>
       <c r="H608" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I608" t="inlineStr">
@@ -27414,7 +27414,7 @@
       <c r="G610" t="inlineStr"/>
       <c r="H610" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I610" t="inlineStr">
@@ -27498,7 +27498,7 @@
       <c r="G612" t="inlineStr"/>
       <c r="H612" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I612" t="inlineStr">
@@ -27540,7 +27540,7 @@
       <c r="G613" t="inlineStr"/>
       <c r="H613" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I613" t="inlineStr">
@@ -27672,7 +27672,7 @@
       <c r="G616" t="inlineStr"/>
       <c r="H616" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I616" t="inlineStr">
@@ -27714,7 +27714,7 @@
       <c r="G617" t="inlineStr"/>
       <c r="H617" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I617" t="inlineStr">
@@ -27804,7 +27804,7 @@
       <c r="G619" t="inlineStr"/>
       <c r="H619" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I619" t="inlineStr">
@@ -27846,7 +27846,7 @@
       <c r="G620" t="inlineStr"/>
       <c r="H620" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I620" t="inlineStr">
@@ -27930,7 +27930,7 @@
       <c r="G622" t="inlineStr"/>
       <c r="H622" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I622" t="inlineStr">
@@ -27972,7 +27972,7 @@
       <c r="G623" t="inlineStr"/>
       <c r="H623" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I623" t="inlineStr">
@@ -28118,7 +28118,7 @@
       <c r="G626" t="inlineStr"/>
       <c r="H626" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I626" t="inlineStr">
@@ -28160,7 +28160,7 @@
       <c r="G627" t="inlineStr"/>
       <c r="H627" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I627" t="inlineStr">
@@ -28250,7 +28250,7 @@
       <c r="G629" t="inlineStr"/>
       <c r="H629" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I629" t="inlineStr">
@@ -28292,7 +28292,7 @@
       <c r="G630" t="inlineStr"/>
       <c r="H630" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I630" t="inlineStr">
@@ -28334,7 +28334,7 @@
       <c r="G631" t="inlineStr"/>
       <c r="H631" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I631" t="inlineStr">
@@ -28424,7 +28424,7 @@
       <c r="G633" t="inlineStr"/>
       <c r="H633" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I633" t="inlineStr">
@@ -28466,7 +28466,7 @@
       <c r="G634" t="inlineStr"/>
       <c r="H634" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I634" t="inlineStr">
@@ -28606,7 +28606,7 @@
       <c r="G637" t="inlineStr"/>
       <c r="H637" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I637" t="inlineStr">
@@ -28648,7 +28648,7 @@
       <c r="G638" t="inlineStr"/>
       <c r="H638" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I638" t="inlineStr">
@@ -28738,7 +28738,7 @@
       <c r="G640" t="inlineStr"/>
       <c r="H640" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I640" t="inlineStr">
@@ -28870,7 +28870,7 @@
       <c r="G643" t="inlineStr"/>
       <c r="H643" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I643" t="inlineStr">
@@ -29058,7 +29058,7 @@
       <c r="G647" t="inlineStr"/>
       <c r="H647" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I647" t="inlineStr">
@@ -29184,7 +29184,7 @@
       <c r="G650" t="inlineStr"/>
       <c r="H650" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I650" t="inlineStr">
@@ -29268,7 +29268,7 @@
       <c r="G652" t="inlineStr"/>
       <c r="H652" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I652" t="inlineStr">
@@ -29394,7 +29394,7 @@
       <c r="G655" t="inlineStr"/>
       <c r="H655" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I655" t="inlineStr">
@@ -29576,7 +29576,7 @@
       <c r="G659" t="inlineStr"/>
       <c r="H659" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I659" t="inlineStr">
@@ -29752,7 +29752,7 @@
       <c r="G663" t="inlineStr"/>
       <c r="H663" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I663" t="inlineStr">
@@ -29836,7 +29836,7 @@
       <c r="G665" t="inlineStr"/>
       <c r="H665" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I665" t="inlineStr">
@@ -29878,7 +29878,7 @@
       <c r="G666" t="inlineStr"/>
       <c r="H666" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I666" t="inlineStr">
@@ -30110,7 +30110,7 @@
       <c r="G671" t="inlineStr"/>
       <c r="H671" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I671" t="inlineStr">
@@ -30152,7 +30152,7 @@
       <c r="G672" t="inlineStr"/>
       <c r="H672" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I672" t="inlineStr">
@@ -30194,7 +30194,7 @@
       <c r="G673" t="inlineStr"/>
       <c r="H673" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I673" t="inlineStr">
@@ -30236,7 +30236,7 @@
       <c r="G674" t="inlineStr"/>
       <c r="H674" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I674" t="inlineStr">
@@ -30278,7 +30278,7 @@
       <c r="G675" t="inlineStr"/>
       <c r="H675" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I675" t="inlineStr">
@@ -30368,7 +30368,7 @@
       <c r="G677" t="inlineStr"/>
       <c r="H677" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I677" t="inlineStr">
@@ -30410,7 +30410,7 @@
       <c r="G678" t="inlineStr"/>
       <c r="H678" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I678" t="inlineStr">
@@ -30452,7 +30452,7 @@
       <c r="G679" t="inlineStr"/>
       <c r="H679" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I679" t="inlineStr">
@@ -30592,7 +30592,7 @@
       <c r="G682" t="inlineStr"/>
       <c r="H682" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I682" t="inlineStr">
@@ -30732,7 +30732,7 @@
       <c r="G685" t="inlineStr"/>
       <c r="H685" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I685" t="inlineStr">
@@ -30774,7 +30774,7 @@
       <c r="G686" t="inlineStr"/>
       <c r="H686" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I686" t="inlineStr">
@@ -30906,7 +30906,7 @@
       <c r="G689" t="inlineStr"/>
       <c r="H689" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I689" t="inlineStr">
@@ -31132,7 +31132,7 @@
       <c r="G694" t="inlineStr"/>
       <c r="H694" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I694" t="inlineStr">
@@ -31264,7 +31264,7 @@
       <c r="G697" t="inlineStr"/>
       <c r="H697" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I697" t="inlineStr">
@@ -31354,7 +31354,7 @@
       <c r="G699" t="inlineStr"/>
       <c r="H699" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I699" t="inlineStr">
@@ -31396,7 +31396,7 @@
       <c r="G700" t="inlineStr"/>
       <c r="H700" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I700" t="inlineStr">
@@ -31480,7 +31480,7 @@
       <c r="G702" t="inlineStr"/>
       <c r="H702" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I702" t="inlineStr">
@@ -31522,7 +31522,7 @@
       <c r="G703" t="inlineStr"/>
       <c r="H703" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I703" t="inlineStr">
@@ -31612,7 +31612,7 @@
       <c r="G705" t="inlineStr"/>
       <c r="H705" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I705" t="inlineStr">
@@ -31654,7 +31654,7 @@
       <c r="G706" t="inlineStr"/>
       <c r="H706" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I706" t="inlineStr">
@@ -31744,7 +31744,7 @@
       <c r="G708" t="inlineStr"/>
       <c r="H708" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I708" t="inlineStr">
@@ -31828,7 +31828,7 @@
       <c r="G710" t="inlineStr"/>
       <c r="H710" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I710" t="inlineStr">
@@ -31968,7 +31968,7 @@
       <c r="G713" t="inlineStr"/>
       <c r="H713" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I713" t="inlineStr">
@@ -32156,7 +32156,7 @@
       <c r="G717" t="inlineStr"/>
       <c r="H717" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I717" t="inlineStr">
@@ -32294,7 +32294,7 @@
       <c r="G720" t="inlineStr"/>
       <c r="H720" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I720" t="inlineStr">
@@ -32384,7 +32384,7 @@
       <c r="G722" t="inlineStr"/>
       <c r="H722" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I722" t="inlineStr">
@@ -32468,7 +32468,7 @@
       <c r="G724" t="inlineStr"/>
       <c r="H724" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I724" t="inlineStr">
@@ -32558,7 +32558,7 @@
       <c r="G726" t="inlineStr"/>
       <c r="H726" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I726" t="inlineStr">
@@ -32690,7 +32690,7 @@
       <c r="G729" t="inlineStr"/>
       <c r="H729" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I729" t="inlineStr">
@@ -32774,7 +32774,7 @@
       <c r="G731" t="inlineStr"/>
       <c r="H731" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I731" t="inlineStr">
@@ -32864,7 +32864,7 @@
       <c r="G733" t="inlineStr"/>
       <c r="H733" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I733" t="inlineStr">
@@ -32954,7 +32954,7 @@
       <c r="G735" t="inlineStr"/>
       <c r="H735" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I735" t="inlineStr">
@@ -33086,7 +33086,7 @@
       <c r="G738" t="inlineStr"/>
       <c r="H738" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I738" t="inlineStr">
@@ -33316,7 +33316,7 @@
       <c r="G743" t="inlineStr"/>
       <c r="H743" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I743" t="inlineStr">
@@ -33504,7 +33504,7 @@
       <c r="G747" t="inlineStr"/>
       <c r="H747" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I747" t="inlineStr">
@@ -33734,7 +33734,7 @@
       <c r="G752" t="inlineStr"/>
       <c r="H752" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I752" t="inlineStr">
@@ -33776,7 +33776,7 @@
       <c r="G753" t="inlineStr"/>
       <c r="H753" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I753" t="inlineStr">
@@ -33818,7 +33818,7 @@
       <c r="G754" t="inlineStr"/>
       <c r="H754" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I754" t="inlineStr">
@@ -33902,7 +33902,7 @@
       <c r="G756" t="inlineStr"/>
       <c r="H756" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I756" t="inlineStr">
@@ -34084,7 +34084,7 @@
       <c r="G760" t="inlineStr"/>
       <c r="H760" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I760" t="inlineStr">
@@ -34266,7 +34266,7 @@
       <c r="G764" t="inlineStr"/>
       <c r="H764" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I764" t="inlineStr">
@@ -34356,7 +34356,7 @@
       <c r="G766" t="inlineStr"/>
       <c r="H766" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I766" t="inlineStr">
@@ -34488,7 +34488,7 @@
       <c r="G769" t="inlineStr"/>
       <c r="H769" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I769" t="inlineStr">
@@ -34620,7 +34620,7 @@
       <c r="G772" t="inlineStr"/>
       <c r="H772" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I772" t="inlineStr">
@@ -34758,7 +34758,7 @@
       <c r="G775" t="inlineStr"/>
       <c r="H775" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I775" t="inlineStr">
@@ -34896,7 +34896,7 @@
       <c r="G778" t="inlineStr"/>
       <c r="H778" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I778" t="inlineStr">
@@ -34938,7 +34938,7 @@
       <c r="G779" t="inlineStr"/>
       <c r="H779" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I779" t="inlineStr">
@@ -34980,7 +34980,7 @@
       <c r="G780" t="inlineStr"/>
       <c r="H780" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I780" t="inlineStr">
@@ -35022,7 +35022,7 @@
       <c r="G781" t="inlineStr"/>
       <c r="H781" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I781" t="inlineStr">
@@ -35112,7 +35112,7 @@
       <c r="G783" t="inlineStr"/>
       <c r="H783" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I783" t="inlineStr">
@@ -35202,7 +35202,7 @@
       <c r="G785" t="inlineStr"/>
       <c r="H785" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I785" t="inlineStr">
@@ -35286,7 +35286,7 @@
       <c r="G787" t="inlineStr"/>
       <c r="H787" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I787" t="inlineStr">
@@ -35370,7 +35370,7 @@
       <c r="G789" t="inlineStr"/>
       <c r="H789" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I789" t="inlineStr">
@@ -35510,7 +35510,7 @@
       <c r="G792" t="inlineStr"/>
       <c r="H792" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I792" t="inlineStr">
@@ -35642,7 +35642,7 @@
       <c r="G795" t="inlineStr"/>
       <c r="H795" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I795" t="inlineStr">
@@ -35774,7 +35774,7 @@
       <c r="G798" t="inlineStr"/>
       <c r="H798" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I798" t="inlineStr">
@@ -35864,7 +35864,7 @@
       <c r="G800" t="inlineStr"/>
       <c r="H800" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I800" t="inlineStr">
@@ -35906,7 +35906,7 @@
       <c r="G801" t="inlineStr"/>
       <c r="H801" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I801" t="inlineStr">
@@ -36082,7 +36082,7 @@
       <c r="G805" t="inlineStr"/>
       <c r="H805" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I805" t="inlineStr">
@@ -36166,7 +36166,7 @@
       <c r="G807" t="inlineStr"/>
       <c r="H807" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I807" t="inlineStr">
@@ -36208,7 +36208,7 @@
       <c r="G808" t="inlineStr"/>
       <c r="H808" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I808" t="inlineStr">
@@ -36342,7 +36342,7 @@
       <c r="G811" t="inlineStr"/>
       <c r="H811" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I811" t="inlineStr">
@@ -36384,7 +36384,7 @@
       <c r="G812" t="inlineStr"/>
       <c r="H812" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I812" t="inlineStr">
@@ -36516,7 +36516,7 @@
       <c r="G815" t="inlineStr"/>
       <c r="H815" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I815" t="inlineStr">
@@ -36600,7 +36600,7 @@
       <c r="G817" t="inlineStr"/>
       <c r="H817" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I817" t="inlineStr">
@@ -36732,7 +36732,7 @@
       <c r="G820" t="inlineStr"/>
       <c r="H820" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I820" t="inlineStr">
@@ -36816,7 +36816,7 @@
       <c r="G822" t="inlineStr"/>
       <c r="H822" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I822" t="inlineStr">
@@ -36956,7 +36956,7 @@
       <c r="G825" t="inlineStr"/>
       <c r="H825" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I825" t="inlineStr">
@@ -36998,7 +36998,7 @@
       <c r="G826" t="inlineStr"/>
       <c r="H826" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I826" t="inlineStr">
@@ -37040,7 +37040,7 @@
       <c r="G827" t="inlineStr"/>
       <c r="H827" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I827" t="inlineStr">
@@ -37082,7 +37082,7 @@
       <c r="G828" t="inlineStr"/>
       <c r="H828" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I828" t="inlineStr">
@@ -37124,7 +37124,7 @@
       <c r="G829" t="inlineStr"/>
       <c r="H829" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I829" t="inlineStr">
@@ -37214,7 +37214,7 @@
       <c r="G831" t="inlineStr"/>
       <c r="H831" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I831" t="inlineStr">
@@ -37438,7 +37438,7 @@
       <c r="G836" t="inlineStr"/>
       <c r="H836" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I836" t="inlineStr">
@@ -37528,7 +37528,7 @@
       <c r="G838" t="inlineStr"/>
       <c r="H838" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I838" t="inlineStr">
@@ -37570,7 +37570,7 @@
       <c r="G839" t="inlineStr"/>
       <c r="H839" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I839" t="inlineStr">
@@ -37660,7 +37660,7 @@
       <c r="G841" t="inlineStr"/>
       <c r="H841" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I841" t="inlineStr">
@@ -37744,7 +37744,7 @@
       <c r="G843" t="inlineStr"/>
       <c r="H843" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I843" t="inlineStr">
@@ -37828,7 +37828,7 @@
       <c r="G845" t="inlineStr"/>
       <c r="H845" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I845" t="inlineStr">
@@ -37870,7 +37870,7 @@
       <c r="G846" t="inlineStr"/>
       <c r="H846" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I846" t="inlineStr">
@@ -37912,7 +37912,7 @@
       <c r="G847" t="inlineStr"/>
       <c r="H847" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I847" t="inlineStr">
@@ -38100,7 +38100,7 @@
       <c r="G851" t="inlineStr"/>
       <c r="H851" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I851" t="inlineStr">
@@ -38142,7 +38142,7 @@
       <c r="G852" t="inlineStr"/>
       <c r="H852" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I852" t="inlineStr">
@@ -38232,7 +38232,7 @@
       <c r="G854" t="inlineStr"/>
       <c r="H854" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I854" t="inlineStr">
@@ -38378,7 +38378,7 @@
       <c r="G857" t="inlineStr"/>
       <c r="H857" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I857" t="inlineStr">
@@ -38602,7 +38602,7 @@
       <c r="G862" t="inlineStr"/>
       <c r="H862" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I862" t="inlineStr">
@@ -38644,7 +38644,7 @@
       <c r="G863" t="inlineStr"/>
       <c r="H863" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I863" t="inlineStr">
@@ -38686,7 +38686,7 @@
       <c r="G864" t="inlineStr"/>
       <c r="H864" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I864" t="inlineStr">
@@ -38776,7 +38776,7 @@
       <c r="G866" t="inlineStr"/>
       <c r="H866" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I866" t="inlineStr">
@@ -38916,7 +38916,7 @@
       <c r="G869" t="inlineStr"/>
       <c r="H869" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I869" t="inlineStr">
@@ -38958,7 +38958,7 @@
       <c r="G870" t="inlineStr"/>
       <c r="H870" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I870" t="inlineStr">
@@ -39084,7 +39084,7 @@
       <c r="G873" t="inlineStr"/>
       <c r="H873" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I873" t="inlineStr">
@@ -39210,7 +39210,7 @@
       <c r="G876" t="inlineStr"/>
       <c r="H876" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I876" t="inlineStr">
@@ -39342,7 +39342,7 @@
       <c r="G879" t="inlineStr"/>
       <c r="H879" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I879" t="inlineStr">
@@ -39480,7 +39480,7 @@
       <c r="G882" t="inlineStr"/>
       <c r="H882" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I882" t="inlineStr">
@@ -39570,7 +39570,7 @@
       <c r="G884" t="inlineStr"/>
       <c r="H884" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I884" t="inlineStr">
@@ -39660,7 +39660,7 @@
       <c r="G886" t="inlineStr"/>
       <c r="H886" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I886" t="inlineStr">
@@ -39786,7 +39786,7 @@
       <c r="G889" t="inlineStr"/>
       <c r="H889" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I889" t="inlineStr">
@@ -40012,7 +40012,7 @@
       <c r="G894" t="inlineStr"/>
       <c r="H894" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I894" t="inlineStr">
@@ -40054,7 +40054,7 @@
       <c r="G895" t="inlineStr"/>
       <c r="H895" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I895" t="inlineStr">
@@ -40096,7 +40096,7 @@
       <c r="G896" t="inlineStr"/>
       <c r="H896" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I896" t="inlineStr">
@@ -40362,7 +40362,7 @@
       <c r="G902" t="inlineStr"/>
       <c r="H902" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I902" t="inlineStr">
@@ -40488,7 +40488,7 @@
       <c r="G905" t="inlineStr"/>
       <c r="H905" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I905" t="inlineStr">
@@ -40620,7 +40620,7 @@
       <c r="G908" t="inlineStr"/>
       <c r="H908" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I908" t="inlineStr">
@@ -40710,7 +40710,7 @@
       <c r="G910" t="inlineStr"/>
       <c r="H910" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I910" t="inlineStr">
@@ -40800,7 +40800,7 @@
       <c r="G912" t="inlineStr"/>
       <c r="H912" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I912" t="inlineStr">
@@ -40842,7 +40842,7 @@
       <c r="G913" t="inlineStr"/>
       <c r="H913" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I913" t="inlineStr">
@@ -40932,7 +40932,7 @@
       <c r="G915" t="inlineStr"/>
       <c r="H915" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I915" t="inlineStr">
@@ -41064,7 +41064,7 @@
       <c r="G918" t="inlineStr"/>
       <c r="H918" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I918" t="inlineStr">
@@ -41252,7 +41252,7 @@
       <c r="G922" t="inlineStr"/>
       <c r="H922" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I922" t="inlineStr">
@@ -41294,7 +41294,7 @@
       <c r="G923" t="inlineStr"/>
       <c r="H923" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I923" t="inlineStr">
@@ -41426,7 +41426,7 @@
       <c r="G926" t="inlineStr"/>
       <c r="H926" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I926" t="inlineStr">
@@ -41468,7 +41468,7 @@
       <c r="G927" t="inlineStr"/>
       <c r="H927" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I927" t="inlineStr">
@@ -41644,7 +41644,7 @@
       <c r="G931" t="inlineStr"/>
       <c r="H931" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I931" t="inlineStr">
@@ -41776,7 +41776,7 @@
       <c r="G934" t="inlineStr"/>
       <c r="H934" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I934" t="inlineStr">
@@ -41914,7 +41914,7 @@
       <c r="G937" t="inlineStr"/>
       <c r="H937" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I937" t="inlineStr">
@@ -41998,7 +41998,7 @@
       <c r="G939" t="inlineStr"/>
       <c r="H939" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I939" t="inlineStr">
@@ -42192,7 +42192,7 @@
       <c r="G943" t="inlineStr"/>
       <c r="H943" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I943" t="inlineStr">
@@ -42324,7 +42324,7 @@
       <c r="G946" t="inlineStr"/>
       <c r="H946" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I946" t="inlineStr">
@@ -42414,7 +42414,7 @@
       <c r="G948" t="inlineStr"/>
       <c r="H948" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I948" t="inlineStr">
@@ -42642,7 +42642,7 @@
       <c r="G953" t="inlineStr"/>
       <c r="H953" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I953" t="inlineStr">
@@ -42836,7 +42836,7 @@
       <c r="G957" t="inlineStr"/>
       <c r="H957" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I957" t="inlineStr">
@@ -42974,7 +42974,7 @@
       <c r="G960" t="inlineStr"/>
       <c r="H960" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I960" t="inlineStr">
@@ -43216,7 +43216,7 @@
       <c r="G965" t="inlineStr"/>
       <c r="H965" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I965" t="inlineStr">
@@ -43354,7 +43354,7 @@
       <c r="G968" t="inlineStr"/>
       <c r="H968" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I968" t="inlineStr">
@@ -43396,7 +43396,7 @@
       <c r="G969" t="inlineStr"/>
       <c r="H969" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I969" t="inlineStr">
@@ -43534,7 +43534,7 @@
       <c r="G972" t="inlineStr"/>
       <c r="H972" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I972" t="inlineStr">
@@ -43720,7 +43720,7 @@
       <c r="G976" t="inlineStr"/>
       <c r="H976" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I976" t="inlineStr">
@@ -44004,7 +44004,7 @@
       <c r="G982" t="inlineStr"/>
       <c r="H982" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I982" t="inlineStr">
@@ -44184,7 +44184,7 @@
       <c r="G986" t="inlineStr"/>
       <c r="H986" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I986" t="inlineStr">
@@ -44364,7 +44364,7 @@
       <c r="G990" t="inlineStr"/>
       <c r="H990" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I990" t="inlineStr">
@@ -44630,7 +44630,7 @@
       <c r="G996" t="inlineStr"/>
       <c r="H996" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I996" t="inlineStr">
@@ -44818,7 +44818,7 @@
       <c r="G1000" t="inlineStr"/>
       <c r="H1000" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1000" t="inlineStr">
@@ -45172,7 +45172,7 @@
       <c r="G1008" t="inlineStr"/>
       <c r="H1008" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1008" t="inlineStr">
@@ -45556,7 +45556,7 @@
       <c r="G1017" t="inlineStr"/>
       <c r="H1017" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1017" t="inlineStr">
@@ -45862,7 +45862,7 @@
       <c r="G1024" t="inlineStr"/>
       <c r="H1024" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1024" t="inlineStr">
@@ -46072,7 +46072,7 @@
       <c r="G1029" t="inlineStr"/>
       <c r="H1029" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1029" t="inlineStr">
@@ -46300,7 +46300,7 @@
       <c r="G1034" t="inlineStr"/>
       <c r="H1034" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1034" t="inlineStr">
@@ -46476,7 +46476,7 @@
       <c r="G1038" t="inlineStr"/>
       <c r="H1038" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1038" t="inlineStr">
@@ -46614,7 +46614,7 @@
       <c r="G1041" t="inlineStr"/>
       <c r="H1041" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1041" t="inlineStr">
@@ -46754,7 +46754,7 @@
       <c r="G1044" t="inlineStr"/>
       <c r="H1044" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1044" t="inlineStr">
@@ -46948,7 +46948,7 @@
       <c r="G1048" t="inlineStr"/>
       <c r="H1048" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1048" t="inlineStr">
@@ -47094,7 +47094,7 @@
       <c r="G1051" t="inlineStr"/>
       <c r="H1051" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1051" t="inlineStr">
@@ -47234,7 +47234,7 @@
       <c r="G1054" t="inlineStr"/>
       <c r="H1054" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1054" t="inlineStr">
@@ -47276,7 +47276,7 @@
       <c r="G1055" t="inlineStr"/>
       <c r="H1055" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1055" t="inlineStr">
@@ -47366,7 +47366,7 @@
       <c r="G1057" t="inlineStr"/>
       <c r="H1057" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1057" t="inlineStr">
@@ -47542,7 +47542,7 @@
       <c r="G1061" t="inlineStr"/>
       <c r="H1061" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1061" t="inlineStr">
@@ -47584,7 +47584,7 @@
       <c r="G1062" t="inlineStr"/>
       <c r="H1062" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1062" t="inlineStr">
@@ -47802,7 +47802,7 @@
       <c r="G1067" t="inlineStr"/>
       <c r="H1067" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1067" t="inlineStr">
@@ -47844,7 +47844,7 @@
       <c r="G1068" t="inlineStr"/>
       <c r="H1068" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1068" t="inlineStr">
@@ -48080,7 +48080,7 @@
       <c r="G1073" t="inlineStr"/>
       <c r="H1073" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1073" t="inlineStr">
@@ -48324,7 +48324,7 @@
       <c r="G1078" t="inlineStr"/>
       <c r="H1078" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1078" t="inlineStr">
@@ -48554,7 +48554,7 @@
       <c r="G1083" t="inlineStr"/>
       <c r="H1083" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1083" t="inlineStr">
@@ -48840,7 +48840,7 @@
       <c r="G1089" t="inlineStr"/>
       <c r="H1089" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1089" t="inlineStr">
@@ -48882,7 +48882,7 @@
       <c r="G1090" t="inlineStr"/>
       <c r="H1090" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1090" t="inlineStr">
@@ -49022,7 +49022,7 @@
       <c r="G1093" t="inlineStr"/>
       <c r="H1093" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1093" t="inlineStr">
@@ -49064,7 +49064,7 @@
       <c r="G1094" t="inlineStr"/>
       <c r="H1094" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1094" t="inlineStr">
@@ -49106,7 +49106,7 @@
       <c r="G1095" t="inlineStr"/>
       <c r="H1095" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1095" t="inlineStr">
@@ -49148,7 +49148,7 @@
       <c r="G1096" t="inlineStr"/>
       <c r="H1096" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1096" t="inlineStr">
@@ -49286,7 +49286,7 @@
       <c r="G1099" t="inlineStr"/>
       <c r="H1099" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1099" t="inlineStr">
@@ -49466,7 +49466,7 @@
       <c r="G1103" t="inlineStr"/>
       <c r="H1103" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1103" t="inlineStr">
@@ -49646,7 +49646,7 @@
       <c r="G1107" t="inlineStr"/>
       <c r="H1107" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1107" t="inlineStr">
@@ -49778,7 +49778,7 @@
       <c r="G1110" t="inlineStr"/>
       <c r="H1110" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1110" t="inlineStr">
@@ -49820,7 +49820,7 @@
       <c r="G1111" t="inlineStr"/>
       <c r="H1111" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1111" t="inlineStr">
@@ -50056,7 +50056,7 @@
       <c r="G1116" t="inlineStr"/>
       <c r="H1116" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1116" t="inlineStr">
@@ -50250,7 +50250,7 @@
       <c r="G1120" t="inlineStr"/>
       <c r="H1120" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1120" t="inlineStr">
@@ -50340,7 +50340,7 @@
       <c r="G1122" t="inlineStr"/>
       <c r="H1122" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1122" t="inlineStr">
@@ -50624,7 +50624,7 @@
       <c r="G1128" t="inlineStr"/>
       <c r="H1128" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1128" t="inlineStr">
@@ -50950,7 +50950,7 @@
       <c r="G1135" t="inlineStr"/>
       <c r="H1135" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1135" t="inlineStr">
@@ -51232,7 +51232,7 @@
       <c r="G1141" t="inlineStr"/>
       <c r="H1141" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1141" t="inlineStr">
@@ -51420,7 +51420,7 @@
       <c r="G1145" t="inlineStr"/>
       <c r="H1145" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1145" t="inlineStr">
@@ -51614,7 +51614,7 @@
       <c r="G1149" t="inlineStr"/>
       <c r="H1149" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1149" t="inlineStr">
@@ -51946,7 +51946,7 @@
       <c r="G1156" t="inlineStr"/>
       <c r="H1156" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1156" t="inlineStr">
@@ -52230,7 +52230,7 @@
       <c r="G1162" t="inlineStr"/>
       <c r="H1162" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1162" t="inlineStr">
@@ -52368,7 +52368,7 @@
       <c r="G1165" t="inlineStr"/>
       <c r="H1165" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1165" t="inlineStr">
@@ -52674,7 +52674,7 @@
       <c r="G1172" t="inlineStr"/>
       <c r="H1172" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1172" t="inlineStr">
@@ -52908,7 +52908,7 @@
       <c r="G1177" t="inlineStr"/>
       <c r="H1177" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1177" t="inlineStr">
@@ -53042,7 +53042,7 @@
       <c r="G1180" t="inlineStr"/>
       <c r="H1180" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1180" t="inlineStr">
@@ -53264,7 +53264,7 @@
       <c r="G1185" t="inlineStr"/>
       <c r="H1185" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1185" t="inlineStr">
@@ -53534,7 +53534,7 @@
       <c r="G1191" t="inlineStr"/>
       <c r="H1191" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1191" t="inlineStr">
@@ -53800,7 +53800,7 @@
       <c r="G1197" t="inlineStr"/>
       <c r="H1197" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1197" t="inlineStr">
@@ -53980,7 +53980,7 @@
       <c r="G1201" t="inlineStr"/>
       <c r="H1201" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1201" t="inlineStr">
@@ -54250,7 +54250,7 @@
       <c r="G1207" t="inlineStr"/>
       <c r="H1207" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1207" t="inlineStr">
@@ -54472,7 +54472,7 @@
       <c r="G1212" t="inlineStr"/>
       <c r="H1212" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1212" t="inlineStr">
@@ -54738,7 +54738,7 @@
       <c r="G1218" t="inlineStr"/>
       <c r="H1218" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1218" t="inlineStr">
@@ -54920,7 +54920,7 @@
       <c r="G1222" t="inlineStr"/>
       <c r="H1222" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1222" t="inlineStr">
@@ -55136,7 +55136,7 @@
       <c r="G1227" t="inlineStr"/>
       <c r="H1227" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1227" t="inlineStr">
@@ -55324,7 +55324,7 @@
       <c r="G1231" t="inlineStr"/>
       <c r="H1231" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1231" t="inlineStr">
@@ -55510,7 +55510,7 @@
       <c r="G1235" t="inlineStr"/>
       <c r="H1235" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1235" t="inlineStr">
@@ -55656,7 +55656,7 @@
       <c r="G1238" t="inlineStr"/>
       <c r="H1238" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1238" t="inlineStr">
@@ -55794,7 +55794,7 @@
       <c r="G1241" t="inlineStr"/>
       <c r="H1241" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1241" t="inlineStr">
@@ -55980,7 +55980,7 @@
       <c r="G1245" t="inlineStr"/>
       <c r="H1245" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1245" t="inlineStr">
@@ -56168,7 +56168,7 @@
       <c r="G1249" t="inlineStr"/>
       <c r="H1249" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1249" t="inlineStr">
@@ -56258,7 +56258,7 @@
       <c r="G1251" t="inlineStr"/>
       <c r="H1251" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1251" t="inlineStr">
@@ -56398,7 +56398,7 @@
       <c r="G1254" t="inlineStr"/>
       <c r="H1254" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1254" t="inlineStr">
@@ -56488,7 +56488,7 @@
       <c r="G1256" t="inlineStr"/>
       <c r="H1256" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1256" t="inlineStr">
@@ -56780,7 +56780,7 @@
       <c r="G1262" t="inlineStr"/>
       <c r="H1262" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1262" t="inlineStr">
@@ -57038,7 +57038,7 @@
       <c r="G1268" t="inlineStr"/>
       <c r="H1268" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1268" t="inlineStr">
@@ -57268,7 +57268,7 @@
       <c r="G1273" t="inlineStr"/>
       <c r="H1273" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1273" t="inlineStr">
@@ -57450,7 +57450,7 @@
       <c r="G1277" t="inlineStr"/>
       <c r="H1277" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1277" t="inlineStr">
@@ -57770,7 +57770,7 @@
       <c r="G1284" t="inlineStr"/>
       <c r="H1284" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1284" t="inlineStr">
@@ -58038,7 +58038,7 @@
       <c r="G1290" t="inlineStr"/>
       <c r="H1290" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1290" t="inlineStr">
@@ -58340,7 +58340,7 @@
       <c r="G1297" t="inlineStr"/>
       <c r="H1297" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1297" t="inlineStr">
@@ -58558,7 +58558,7 @@
       <c r="G1302" t="inlineStr"/>
       <c r="H1302" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1302" t="inlineStr">
@@ -58952,7 +58952,7 @@
       <c r="G1311" t="inlineStr"/>
       <c r="H1311" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1311" t="inlineStr">
@@ -59472,7 +59472,7 @@
       <c r="G1323" t="inlineStr"/>
       <c r="H1323" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1323" t="inlineStr">
@@ -59606,7 +59606,7 @@
       <c r="G1326" t="inlineStr"/>
       <c r="H1326" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1326" t="inlineStr">
@@ -59740,7 +59740,7 @@
       <c r="G1329" t="inlineStr"/>
       <c r="H1329" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1329" t="inlineStr">
@@ -59866,7 +59866,7 @@
       <c r="G1332" t="inlineStr"/>
       <c r="H1332" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1332" t="inlineStr">
@@ -60000,7 +60000,7 @@
       <c r="G1335" t="inlineStr"/>
       <c r="H1335" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1335" t="inlineStr">
@@ -60176,7 +60176,7 @@
       <c r="G1339" t="inlineStr"/>
       <c r="H1339" t="inlineStr">
         <is>
-          <t>link</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1339" t="inlineStr">
@@ -60218,7 +60218,7 @@
       <c r="G1340" t="inlineStr"/>
       <c r="H1340" t="inlineStr">
         <is>
-          <t>sink</t>
+          <t>road</t>
         </is>
       </c>
       <c r="I1340" t="inlineStr">

</xml_diff>